<commit_message>
add comment for how to insert data as int rather than string
</commit_message>
<xml_diff>
--- a/data/Scrubbed Data.xlsx
+++ b/data/Scrubbed Data.xlsx
@@ -1,19 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guysbryant\Code\Personal\learn_ruby_spreadsheets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF1D315-7CEC-4755-B788-CC175706E3EC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="25396" windowHeight="15346" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="25396" windowHeight="15346" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69" count="69">
   <si>
     <t>MODEL</t>
   </si>
@@ -242,41 +241,41 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\$#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color rgb="FF0070C0"/>
+      <sz val="11"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="16"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1855,7 +1854,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16" count="0"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -2091,7 +2090,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="16200000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -2120,7 +2119,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -2129,7 +2128,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -2138,7 +2137,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -2254,14 +2253,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3">
   <dimension ref="A1:AD32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="3" width="11.53125"/>
     <col min="4" max="4" width="11.53125" style="37"/>
@@ -2277,7 +2276,7 @@
     <col min="27" max="1025" width="11.53125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:30" s="12" customFormat="1" ht="13.9">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2313,7 +2312,7 @@
       <c r="AC1" s="8"/>
       <c r="AD1" s="11"/>
     </row>
-    <row r="2" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2375,12 +2374,12 @@
       <c r="AC2" s="21"/>
       <c r="AD2" s="22"/>
     </row>
-    <row r="3" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="35">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>11</v>
@@ -2437,7 +2436,7 @@
       <c r="AC3" s="21"/>
       <c r="AD3" s="22"/>
     </row>
-    <row r="4" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" s="12" customFormat="1" ht="20.1" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2499,7 +2498,7 @@
       <c r="AC4" s="21"/>
       <c r="AD4" s="22"/>
     </row>
-    <row r="5" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2561,7 +2560,7 @@
       <c r="AC5" s="21"/>
       <c r="AD5" s="22"/>
     </row>
-    <row r="6" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2623,7 +2622,7 @@
       <c r="AC6" s="21"/>
       <c r="AD6" s="22"/>
     </row>
-    <row r="7" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" s="12" customFormat="1" ht="20.1" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2685,7 +2684,7 @@
       <c r="AC7" s="21"/>
       <c r="AD7" s="22"/>
     </row>
-    <row r="8" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2747,7 +2746,7 @@
       <c r="AC8" s="21"/>
       <c r="AD8" s="22"/>
     </row>
-    <row r="9" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2809,7 +2808,7 @@
       <c r="AC9" s="21"/>
       <c r="AD9" s="22"/>
     </row>
-    <row r="10" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" s="12" customFormat="1" ht="20.1" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2871,7 +2870,7 @@
       <c r="AC10" s="21"/>
       <c r="AD10" s="22"/>
     </row>
-    <row r="11" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" s="12" customFormat="1" ht="20.1" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2933,7 +2932,7 @@
       <c r="AC11" s="21"/>
       <c r="AD11" s="22"/>
     </row>
-    <row r="12" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2995,7 +2994,7 @@
       <c r="AC12" s="21"/>
       <c r="AD12" s="22"/>
     </row>
-    <row r="13" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3057,7 +3056,7 @@
       <c r="AC13" s="21"/>
       <c r="AD13" s="22"/>
     </row>
-    <row r="14" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" s="12" customFormat="1" ht="13.9">
       <c r="A14" s="1"/>
       <c r="B14" s="23">
         <v>3854.12</v>
@@ -3107,7 +3106,7 @@
       <c r="AC14" s="29"/>
       <c r="AD14" s="31"/>
     </row>
-    <row r="15" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:30" s="12" customFormat="1" ht="13.9">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -3143,7 +3142,7 @@
       <c r="AC15" s="8"/>
       <c r="AD15" s="11"/>
     </row>
-    <row r="16" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" s="12" customFormat="1" ht="20.1" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -3205,7 +3204,7 @@
       <c r="AC16" s="21"/>
       <c r="AD16" s="22"/>
     </row>
-    <row r="17" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -3269,7 +3268,7 @@
       <c r="AC17" s="21"/>
       <c r="AD17" s="22"/>
     </row>
-    <row r="18" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:30" s="12" customFormat="1" ht="13.9">
       <c r="A18" s="1"/>
       <c r="B18" s="23">
         <v>582.34</v>
@@ -3319,7 +3318,7 @@
       <c r="AC18" s="29"/>
       <c r="AD18" s="31"/>
     </row>
-    <row r="19" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:30" s="12" customFormat="1" ht="13.9">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -3355,7 +3354,7 @@
       <c r="AC19" s="8"/>
       <c r="AD19" s="11"/>
     </row>
-    <row r="20" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -3417,7 +3416,7 @@
       <c r="AC20" s="21"/>
       <c r="AD20" s="22"/>
     </row>
-    <row r="21" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:30" s="12" customFormat="1" ht="13.9">
       <c r="A21" s="1"/>
       <c r="B21" s="23">
         <v>646.96</v>
@@ -3467,7 +3466,7 @@
       <c r="AC21" s="29"/>
       <c r="AD21" s="31"/>
     </row>
-    <row r="22" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:30" s="12" customFormat="1" ht="13.9">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -3503,7 +3502,7 @@
       <c r="AC22" s="8"/>
       <c r="AD22" s="11"/>
     </row>
-    <row r="23" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -3565,7 +3564,7 @@
       <c r="AC23" s="21"/>
       <c r="AD23" s="22"/>
     </row>
-    <row r="24" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3627,7 +3626,7 @@
       <c r="AC24" s="21"/>
       <c r="AD24" s="22"/>
     </row>
-    <row r="25" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -3691,7 +3690,7 @@
       <c r="AC25" s="21"/>
       <c r="AD25" s="22"/>
     </row>
-    <row r="26" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:30" s="12" customFormat="1" ht="13.9">
       <c r="A26" s="1"/>
       <c r="B26" s="23">
         <v>1055.26</v>
@@ -3741,7 +3740,7 @@
       <c r="AC26" s="29"/>
       <c r="AD26" s="31"/>
     </row>
-    <row r="27" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:30" s="12" customFormat="1" ht="13.9">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -3777,7 +3776,7 @@
       <c r="AC27" s="8"/>
       <c r="AD27" s="11"/>
     </row>
-    <row r="28" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -3829,7 +3828,7 @@
       <c r="AC28" s="33"/>
       <c r="AD28" s="22"/>
     </row>
-    <row r="29" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:30" s="12" customFormat="1" ht="20.1" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -3863,7 +3862,7 @@
       <c r="AC29" s="33"/>
       <c r="AD29" s="22"/>
     </row>
-    <row r="30" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -3897,7 +3896,7 @@
       <c r="AC30" s="33"/>
       <c r="AD30" s="22"/>
     </row>
-    <row r="31" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -3931,7 +3930,7 @@
       <c r="AC31" s="33"/>
       <c r="AD31" s="22"/>
     </row>
-    <row r="32" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:30" s="12" customFormat="1" ht="20.1" customHeight="1">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -4472,7 +4471,7 @@
       <formula>AND(TODAY()-FLOOR(P31,1)&lt;=6,FLOOR(P31,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>

</xml_diff>

<commit_message>
add blank line with fill color set to black
</commit_message>
<xml_diff>
--- a/data/Scrubbed Data.xlsx
+++ b/data/Scrubbed Data.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guysbryant\Code\Personal\learn_ruby_spreadsheets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F5092A-3E09-487D-ACB3-01B6639DB373}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="25396" windowHeight="15346" tabRatio="500"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="25396" windowHeight="15346" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69" count="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="69">
   <si>
     <t>MODEL</t>
   </si>
@@ -241,41 +243,41 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\$#,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Arial"/>
       <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF0070C0"/>
-      <sz val="11"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <color rgb="FFFF0000"/>
-      <sz val="11"/>
     </font>
     <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="16"/>
     </font>
   </fonts>
   <fills count="4">
@@ -367,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -468,6 +470,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1854,7 +1859,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16" count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -2090,7 +2095,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="false"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -2119,7 +2124,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="false">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -2128,7 +2133,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="false">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -2137,7 +2142,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="false">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -2253,14 +2258,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="Y30" sqref="Y30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="11.53125"/>
     <col min="4" max="4" width="11.53125" style="37"/>
@@ -2276,7 +2281,7 @@
     <col min="27" max="1025" width="11.53125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="12" customFormat="1" ht="13.9">
+    <row r="1" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2312,7 +2317,7 @@
       <c r="AC1" s="8"/>
       <c r="AD1" s="11"/>
     </row>
-    <row r="2" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="2" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2365,7 +2370,7 @@
         <v>10</v>
       </c>
       <c r="Y2" s="13" t="str">
-        <f t="shared" ref="Y2:Y13" si="0">CONCATENATE(T2,".",U2,".",V2,W2,".",X2)</f>
+        <f t="shared" ref="Y2:Y14" si="0">CONCATENATE(T2,".",U2,".",V2,W2,".",X2)</f>
         <v>serial1.line01.as1qa1.S</v>
       </c>
       <c r="Z2" s="13"/>
@@ -2374,7 +2379,7 @@
       <c r="AC2" s="21"/>
       <c r="AD2" s="22"/>
     </row>
-    <row r="3" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="3" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2398,7 +2403,7 @@
       </c>
       <c r="L3" s="17">
         <f t="shared" ref="L3:L13" si="1">PRODUCT(D3, K3)</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="M3" s="13"/>
       <c r="N3" s="18" t="s">
@@ -2436,7 +2441,7 @@
       <c r="AC3" s="21"/>
       <c r="AD3" s="22"/>
     </row>
-    <row r="4" spans="1:30" s="12" customFormat="1" ht="20.1" customHeight="1">
+    <row r="4" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2498,7 +2503,7 @@
       <c r="AC4" s="21"/>
       <c r="AD4" s="22"/>
     </row>
-    <row r="5" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="5" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2560,7 +2565,7 @@
       <c r="AC5" s="21"/>
       <c r="AD5" s="22"/>
     </row>
-    <row r="6" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="6" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2622,7 +2627,7 @@
       <c r="AC6" s="21"/>
       <c r="AD6" s="22"/>
     </row>
-    <row r="7" spans="1:30" s="12" customFormat="1" ht="20.1" customHeight="1">
+    <row r="7" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2684,7 +2689,7 @@
       <c r="AC7" s="21"/>
       <c r="AD7" s="22"/>
     </row>
-    <row r="8" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="8" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2746,7 +2751,7 @@
       <c r="AC8" s="21"/>
       <c r="AD8" s="22"/>
     </row>
-    <row r="9" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="9" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2808,7 +2813,7 @@
       <c r="AC9" s="21"/>
       <c r="AD9" s="22"/>
     </row>
-    <row r="10" spans="1:30" s="12" customFormat="1" ht="20.1" customHeight="1">
+    <row r="10" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2870,7 +2875,7 @@
       <c r="AC10" s="21"/>
       <c r="AD10" s="22"/>
     </row>
-    <row r="11" spans="1:30" s="12" customFormat="1" ht="20.1" customHeight="1">
+    <row r="11" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2932,7 +2937,7 @@
       <c r="AC11" s="21"/>
       <c r="AD11" s="22"/>
     </row>
-    <row r="12" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="12" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2994,7 +2999,7 @@
       <c r="AC12" s="21"/>
       <c r="AD12" s="22"/>
     </row>
-    <row r="13" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="13" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3056,7 +3061,7 @@
       <c r="AC13" s="21"/>
       <c r="AD13" s="22"/>
     </row>
-    <row r="14" spans="1:30" s="12" customFormat="1" ht="13.9">
+    <row r="14" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="23">
         <v>3854.12</v>
@@ -3066,7 +3071,7 @@
       </c>
       <c r="D14" s="36">
         <f>SUM(D2:D13)</f>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E14" s="24" t="s">
         <v>48</v>
@@ -3097,8 +3102,9 @@
       <c r="V14" s="24"/>
       <c r="W14" s="24"/>
       <c r="X14" s="24"/>
-      <c r="Y14" s="24" t="s">
-        <v>51</v>
+      <c r="Y14" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>...</v>
       </c>
       <c r="Z14" s="24"/>
       <c r="AA14" s="24"/>
@@ -3106,7 +3112,7 @@
       <c r="AC14" s="29"/>
       <c r="AD14" s="31"/>
     </row>
-    <row r="15" spans="1:30" s="12" customFormat="1" ht="13.9">
+    <row r="15" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.4">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -3142,7 +3148,7 @@
       <c r="AC15" s="8"/>
       <c r="AD15" s="11"/>
     </row>
-    <row r="16" spans="1:30" s="12" customFormat="1" ht="20.1" customHeight="1">
+    <row r="16" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -3204,7 +3210,7 @@
       <c r="AC16" s="21"/>
       <c r="AD16" s="22"/>
     </row>
-    <row r="17" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="17" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -3268,7 +3274,7 @@
       <c r="AC17" s="21"/>
       <c r="AD17" s="22"/>
     </row>
-    <row r="18" spans="1:30" s="12" customFormat="1" ht="13.9">
+    <row r="18" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="23">
         <v>582.34</v>
@@ -3309,8 +3315,9 @@
       <c r="V18" s="24"/>
       <c r="W18" s="24"/>
       <c r="X18" s="24"/>
-      <c r="Y18" s="24" t="s">
-        <v>51</v>
+      <c r="Y18" s="40" t="str">
+        <f t="shared" ref="Y18" si="3">CONCATENATE(T18,".",U18,".",V18,W18,".",X18)</f>
+        <v>...</v>
       </c>
       <c r="Z18" s="24"/>
       <c r="AA18" s="24"/>
@@ -3318,7 +3325,7 @@
       <c r="AC18" s="29"/>
       <c r="AD18" s="31"/>
     </row>
-    <row r="19" spans="1:30" s="12" customFormat="1" ht="13.9">
+    <row r="19" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.4">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -3354,7 +3361,7 @@
       <c r="AC19" s="8"/>
       <c r="AD19" s="11"/>
     </row>
-    <row r="20" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="20" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -3377,7 +3384,7 @@
         <v>50</v>
       </c>
       <c r="L20" s="17">
-        <f t="shared" ref="L20" si="3">PRODUCT(D20, K20)</f>
+        <f t="shared" ref="L20" si="4">PRODUCT(D20, K20)</f>
         <v>100</v>
       </c>
       <c r="M20" s="13"/>
@@ -3416,7 +3423,7 @@
       <c r="AC20" s="21"/>
       <c r="AD20" s="22"/>
     </row>
-    <row r="21" spans="1:30" s="12" customFormat="1" ht="13.9">
+    <row r="21" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="23">
         <v>646.96</v>
@@ -3457,8 +3464,9 @@
       <c r="V21" s="24"/>
       <c r="W21" s="24"/>
       <c r="X21" s="24"/>
-      <c r="Y21" s="24" t="s">
-        <v>51</v>
+      <c r="Y21" s="40" t="str">
+        <f t="shared" ref="Y21" si="5">CONCATENATE(T21,".",U21,".",V21,W21,".",X21)</f>
+        <v>...</v>
       </c>
       <c r="Z21" s="24"/>
       <c r="AA21" s="24"/>
@@ -3466,7 +3474,7 @@
       <c r="AC21" s="29"/>
       <c r="AD21" s="31"/>
     </row>
-    <row r="22" spans="1:30" s="12" customFormat="1" ht="13.9">
+    <row r="22" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.4">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -3502,7 +3510,7 @@
       <c r="AC22" s="8"/>
       <c r="AD22" s="11"/>
     </row>
-    <row r="23" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="23" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -3525,7 +3533,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="17">
-        <f t="shared" ref="L23:L25" si="4">PRODUCT(D23, K23)</f>
+        <f t="shared" ref="L23:L25" si="6">PRODUCT(D23, K23)</f>
         <v>80</v>
       </c>
       <c r="M23" s="13"/>
@@ -3564,7 +3572,7 @@
       <c r="AC23" s="21"/>
       <c r="AD23" s="22"/>
     </row>
-    <row r="24" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="24" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3587,7 +3595,7 @@
         <v>30</v>
       </c>
       <c r="L24" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="M24" s="13"/>
@@ -3626,7 +3634,7 @@
       <c r="AC24" s="21"/>
       <c r="AD24" s="22"/>
     </row>
-    <row r="25" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="25" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -3649,7 +3657,7 @@
         <v>50</v>
       </c>
       <c r="L25" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="M25" s="13"/>
@@ -3690,7 +3698,7 @@
       <c r="AC25" s="21"/>
       <c r="AD25" s="22"/>
     </row>
-    <row r="26" spans="1:30" s="12" customFormat="1" ht="13.9">
+    <row r="26" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="23">
         <v>1055.26</v>
@@ -3731,8 +3739,9 @@
       <c r="V26" s="24"/>
       <c r="W26" s="24"/>
       <c r="X26" s="24"/>
-      <c r="Y26" s="24" t="s">
-        <v>51</v>
+      <c r="Y26" s="40" t="str">
+        <f t="shared" ref="Y26" si="7">CONCATENATE(T26,".",U26,".",V26,W26,".",X26)</f>
+        <v>...</v>
       </c>
       <c r="Z26" s="24"/>
       <c r="AA26" s="24"/>
@@ -3740,7 +3749,7 @@
       <c r="AC26" s="29"/>
       <c r="AD26" s="31"/>
     </row>
-    <row r="27" spans="1:30" s="12" customFormat="1" ht="13.9">
+    <row r="27" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.4">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -3776,7 +3785,7 @@
       <c r="AC27" s="8"/>
       <c r="AD27" s="11"/>
     </row>
-    <row r="28" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="28" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -3800,7 +3809,7 @@
         <v>10</v>
       </c>
       <c r="L28" s="38">
-        <f t="shared" ref="L28" si="5">PRODUCT(D28, K28)</f>
+        <f t="shared" ref="L28" si="8">PRODUCT(D28, K28)</f>
         <v>60</v>
       </c>
       <c r="M28" s="24"/>
@@ -3819,8 +3828,9 @@
       <c r="V28" s="24"/>
       <c r="W28" s="24"/>
       <c r="X28" s="24"/>
-      <c r="Y28" s="24" t="s">
-        <v>51</v>
+      <c r="Y28" s="40" t="str">
+        <f t="shared" ref="Y28:Y32" si="9">CONCATENATE(T28,".",U28,".",V28,W28,".",X28)</f>
+        <v>...</v>
       </c>
       <c r="Z28" s="24"/>
       <c r="AA28" s="24"/>
@@ -3828,7 +3838,7 @@
       <c r="AC28" s="33"/>
       <c r="AD28" s="22"/>
     </row>
-    <row r="29" spans="1:30" s="12" customFormat="1" ht="20.1" customHeight="1">
+    <row r="29" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -3853,8 +3863,9 @@
       <c r="V29" s="24"/>
       <c r="W29" s="24"/>
       <c r="X29" s="24"/>
-      <c r="Y29" s="24" t="s">
-        <v>51</v>
+      <c r="Y29" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>...</v>
       </c>
       <c r="Z29" s="24"/>
       <c r="AA29" s="24"/>
@@ -3862,7 +3873,7 @@
       <c r="AC29" s="33"/>
       <c r="AD29" s="22"/>
     </row>
-    <row r="30" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="30" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -3887,8 +3898,9 @@
       <c r="V30" s="24"/>
       <c r="W30" s="24"/>
       <c r="X30" s="24"/>
-      <c r="Y30" s="24" t="s">
-        <v>51</v>
+      <c r="Y30" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>...</v>
       </c>
       <c r="Z30" s="24"/>
       <c r="AA30" s="24"/>
@@ -3896,7 +3908,7 @@
       <c r="AC30" s="33"/>
       <c r="AD30" s="22"/>
     </row>
-    <row r="31" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="31" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -3921,8 +3933,9 @@
       <c r="V31" s="24"/>
       <c r="W31" s="24"/>
       <c r="X31" s="24"/>
-      <c r="Y31" s="24" t="s">
-        <v>51</v>
+      <c r="Y31" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>...</v>
       </c>
       <c r="Z31" s="24"/>
       <c r="AA31" s="24"/>
@@ -3930,7 +3943,7 @@
       <c r="AC31" s="33"/>
       <c r="AD31" s="22"/>
     </row>
-    <row r="32" spans="1:30" s="12" customFormat="1" ht="20.1" customHeight="1">
+    <row r="32" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -3955,8 +3968,9 @@
       <c r="V32" s="24"/>
       <c r="W32" s="24"/>
       <c r="X32" s="24"/>
-      <c r="Y32" s="24" t="s">
-        <v>51</v>
+      <c r="Y32" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>...</v>
       </c>
       <c r="Z32" s="24"/>
       <c r="AA32" s="24"/>
@@ -4471,7 +4485,7 @@
       <formula>AND(TODAY()-FLOOR(P31,1)&lt;=6,FLOOR(P31,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>

</xml_diff>

<commit_message>
add another line to Scrubbed Data to work on getting combined qty for total row
</commit_message>
<xml_diff>
--- a/data/Scrubbed Data.xlsx
+++ b/data/Scrubbed Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guysbryant\Code\Personal\learn_ruby_spreadsheets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F5092A-3E09-487D-ACB3-01B6639DB373}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CD0B33-FA53-4C64-8366-6FB574E1C446}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="25396" windowHeight="15346" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="68">
   <si>
     <t>MODEL</t>
   </si>
@@ -184,9 +184,6 @@
   </si>
   <si>
     <t>TOTAL EXTENDED</t>
-  </si>
-  <si>
-    <t>...</t>
   </si>
   <si>
     <t>customer6</t>
@@ -2261,8 +2258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="Y30" sqref="Y30"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -3156,11 +3153,11 @@
         <v>1</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
@@ -3176,7 +3173,7 @@
       </c>
       <c r="M16" s="13"/>
       <c r="N16" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O16" s="18"/>
       <c r="P16" s="19">
@@ -3186,7 +3183,7 @@
       <c r="R16" s="18"/>
       <c r="S16" s="13"/>
       <c r="T16" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U16" s="13" t="s">
         <v>7</v>
@@ -3222,7 +3219,7 @@
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
@@ -3238,7 +3235,7 @@
       </c>
       <c r="M17" s="13"/>
       <c r="N17" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O17" s="18"/>
       <c r="P17" s="19">
@@ -3246,11 +3243,11 @@
       </c>
       <c r="Q17" s="18"/>
       <c r="R17" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S17" s="13"/>
       <c r="T17" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U17" s="13" t="s">
         <v>15</v>
@@ -3373,7 +3370,7 @@
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
@@ -3399,7 +3396,7 @@
       <c r="R20" s="18"/>
       <c r="S20" s="13"/>
       <c r="T20" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U20" s="13" t="s">
         <v>7</v>
@@ -3522,7 +3519,7 @@
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
@@ -3548,7 +3545,7 @@
       <c r="R23" s="18"/>
       <c r="S23" s="13"/>
       <c r="T23" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U23" s="13" t="s">
         <v>7</v>
@@ -3584,7 +3581,7 @@
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
@@ -3610,7 +3607,7 @@
       <c r="R24" s="18"/>
       <c r="S24" s="13"/>
       <c r="T24" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U24" s="13" t="s">
         <v>15</v>
@@ -3646,7 +3643,7 @@
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
@@ -3662,7 +3659,7 @@
       </c>
       <c r="M25" s="13"/>
       <c r="N25" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O25" s="18"/>
       <c r="P25" s="19">
@@ -3670,11 +3667,11 @@
       </c>
       <c r="Q25" s="18"/>
       <c r="R25" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="S25" s="13"/>
       <c r="T25" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U25" s="13" t="s">
         <v>20</v>
@@ -3790,15 +3787,14 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="36">
-        <f>SUM(D26:D26)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F28" s="25"/>
       <c r="G28" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H28" s="26"/>
       <c r="I28" s="26"/>
@@ -3809,8 +3805,8 @@
         <v>10</v>
       </c>
       <c r="L28" s="38">
-        <f t="shared" ref="L28" si="8">PRODUCT(D28, K28)</f>
-        <v>60</v>
+        <f t="shared" ref="L28:L29" si="8">PRODUCT(D28, K28)</f>
+        <v>30</v>
       </c>
       <c r="M28" s="24"/>
       <c r="N28" s="29" t="s">
@@ -3842,19 +3838,36 @@
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="24"/>
+      <c r="D29" s="36">
+        <v>2</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>11</v>
+      </c>
       <c r="F29" s="25"/>
-      <c r="G29" s="24"/>
+      <c r="G29" s="24" t="s">
+        <v>67</v>
+      </c>
       <c r="H29" s="26"/>
       <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="28"/>
+      <c r="J29" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K29" s="27">
+        <v>30</v>
+      </c>
+      <c r="L29" s="38">
+        <f t="shared" si="8"/>
+        <v>60</v>
+      </c>
       <c r="M29" s="24"/>
-      <c r="N29" s="29"/>
+      <c r="N29" s="29" t="s">
+        <v>28</v>
+      </c>
       <c r="O29" s="29"/>
-      <c r="P29" s="32"/>
+      <c r="P29" s="32">
+        <v>43451</v>
+      </c>
       <c r="Q29" s="29"/>
       <c r="R29" s="29"/>
       <c r="S29" s="24"/>

</xml_diff>

<commit_message>
Data changes not important
</commit_message>
<xml_diff>
--- a/data/Scrubbed Data.xlsx
+++ b/data/Scrubbed Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guysbryant\Code\Personal\learn_ruby_spreadsheets\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guysbryant/code/Personal/learn_ruby_spreadsheets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CD0B33-FA53-4C64-8366-6FB574E1C446}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8416775-2DDE-774C-A780-662E472C0EBE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="25396" windowHeight="15346" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>model01</t>
   </si>
   <si>
-    <t>serial1</t>
-  </si>
-  <si>
     <t>line01</t>
   </si>
   <si>
@@ -195,9 +192,6 @@
     <t>model11</t>
   </si>
   <si>
-    <t>serial2</t>
-  </si>
-  <si>
     <t>po14</t>
   </si>
   <si>
@@ -210,15 +204,9 @@
     <t>po15</t>
   </si>
   <si>
-    <t>serial3</t>
-  </si>
-  <si>
     <t>po16</t>
   </si>
   <si>
-    <t>serial4</t>
-  </si>
-  <si>
     <t>po17</t>
   </si>
   <si>
@@ -235,6 +223,18 @@
   </si>
   <si>
     <t>po19</t>
+  </si>
+  <si>
+    <t>workorder1</t>
+  </si>
+  <si>
+    <t>workorder2</t>
+  </si>
+  <si>
+    <t>workorder3</t>
+  </si>
+  <si>
+    <t>workorder4</t>
   </si>
 </sst>
 </file>
@@ -277,7 +277,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,6 +293,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC5E0B4"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
@@ -435,9 +441,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -468,6 +471,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2258,31 +2264,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="S29" sqref="S29"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="11.53125"/>
-    <col min="4" max="4" width="11.53125" style="37"/>
-    <col min="5" max="13" width="11.53125"/>
+    <col min="1" max="3" width="11.5"/>
+    <col min="4" max="4" width="11.5" style="36"/>
+    <col min="5" max="13" width="11.5"/>
     <col min="14" max="14" width="25.6640625" customWidth="1"/>
     <col min="15" max="15" width="24.33203125" customWidth="1"/>
-    <col min="16" max="16" width="15.1328125" customWidth="1"/>
-    <col min="17" max="22" width="11.53125"/>
-    <col min="23" max="23" width="18.19921875" customWidth="1"/>
-    <col min="24" max="24" width="11.46484375" customWidth="1"/>
+    <col min="16" max="16" width="15.1640625" customWidth="1"/>
+    <col min="17" max="22" width="11.5"/>
+    <col min="23" max="23" width="18.1640625" customWidth="1"/>
+    <col min="24" max="24" width="11.5" customWidth="1"/>
     <col min="25" max="25" width="28.6640625" customWidth="1"/>
-    <col min="26" max="26" width="16.1328125" customWidth="1"/>
-    <col min="27" max="1025" width="11.53125"/>
+    <col min="26" max="26" width="16.1640625" customWidth="1"/>
+    <col min="27" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:30" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="34"/>
+      <c r="D1" s="33"/>
       <c r="E1" s="3"/>
       <c r="F1" s="4"/>
       <c r="G1" s="3"/>
@@ -2314,11 +2320,11 @@
       <c r="AC1" s="8"/>
       <c r="AD1" s="11"/>
     </row>
-    <row r="2" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="35">
+      <c r="D2" s="34">
         <v>30</v>
       </c>
       <c r="E2" s="13" t="s">
@@ -2352,23 +2358,23 @@
       <c r="R2" s="18"/>
       <c r="S2" s="13"/>
       <c r="T2" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="U2" s="13" t="s">
+      <c r="V2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="V2" s="13" t="s">
+      <c r="W2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="X2" s="13" t="s">
         <v>9</v>
-      </c>
-      <c r="X2" s="13" t="s">
-        <v>10</v>
       </c>
       <c r="Y2" s="13" t="str">
         <f t="shared" ref="Y2:Y14" si="0">CONCATENATE(T2,".",U2,".",V2,W2,".",X2)</f>
-        <v>serial1.line01.as1qa1.S</v>
+        <v>workorder1.line01.as1qa1.S</v>
       </c>
       <c r="Z2" s="13"/>
       <c r="AA2" s="13"/>
@@ -2376,24 +2382,24 @@
       <c r="AC2" s="21"/>
       <c r="AD2" s="22"/>
     </row>
-    <row r="3" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="35">
+      <c r="D3" s="34">
         <v>4</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
       <c r="J3" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K3" s="16">
         <v>20</v>
@@ -2404,7 +2410,7 @@
       </c>
       <c r="M3" s="13"/>
       <c r="N3" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O3" s="18"/>
       <c r="P3" s="19">
@@ -2414,23 +2420,23 @@
       <c r="R3" s="18"/>
       <c r="S3" s="13"/>
       <c r="T3" s="20" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="U3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="V3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="W3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="X3" s="13" t="s">
         <v>15</v>
-      </c>
-      <c r="V3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="W3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="X3" s="13" t="s">
-        <v>16</v>
       </c>
       <c r="Y3" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>serial1.line02.as1qa1.U.S</v>
+        <v>workorder1.line02.as1qa1.U.S</v>
       </c>
       <c r="Z3" s="13"/>
       <c r="AA3" s="13"/>
@@ -2438,19 +2444,19 @@
       <c r="AC3" s="21"/>
       <c r="AD3" s="22"/>
     </row>
-    <row r="4" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" s="12" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="35">
+      <c r="D4" s="34">
         <v>1</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
@@ -2466,7 +2472,7 @@
       </c>
       <c r="M4" s="13"/>
       <c r="N4" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O4" s="18"/>
       <c r="P4" s="19">
@@ -2476,23 +2482,23 @@
       <c r="R4" s="18"/>
       <c r="S4" s="13"/>
       <c r="T4" s="20" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="U4" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="V4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="W4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="W4" s="13" t="s">
-        <v>9</v>
-      </c>
       <c r="X4" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Y4" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>serial1.line03.as1qa1.U.S</v>
+        <v>workorder1.line03.as1qa1.U.S</v>
       </c>
       <c r="Z4" s="13"/>
       <c r="AA4" s="13"/>
@@ -2500,19 +2506,19 @@
       <c r="AC4" s="21"/>
       <c r="AD4" s="22"/>
     </row>
-    <row r="5" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="35">
+      <c r="D5" s="34">
         <v>1</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
@@ -2528,7 +2534,7 @@
       </c>
       <c r="M5" s="13"/>
       <c r="N5" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O5" s="18"/>
       <c r="P5" s="19">
@@ -2538,23 +2544,23 @@
       <c r="R5" s="18"/>
       <c r="S5" s="13"/>
       <c r="T5" s="20" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="U5" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="W5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="W5" s="13" t="s">
-        <v>9</v>
-      </c>
       <c r="X5" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Y5" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>serial1.line04.as1qa1.U.S</v>
+        <v>workorder1.line04.as1qa1.U.S</v>
       </c>
       <c r="Z5" s="13"/>
       <c r="AA5" s="13"/>
@@ -2562,19 +2568,19 @@
       <c r="AC5" s="21"/>
       <c r="AD5" s="22"/>
     </row>
-    <row r="6" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="35">
+      <c r="D6" s="34">
         <v>1</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
@@ -2590,7 +2596,7 @@
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O6" s="18"/>
       <c r="P6" s="19">
@@ -2600,23 +2606,23 @@
       <c r="R6" s="18"/>
       <c r="S6" s="13"/>
       <c r="T6" s="20" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="U6" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="V6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="W6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="W6" s="13" t="s">
-        <v>9</v>
-      </c>
       <c r="X6" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Y6" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>serial1.line05.as1qa1.U.S</v>
+        <v>workorder1.line05.as1qa1.U.S</v>
       </c>
       <c r="Z6" s="13"/>
       <c r="AA6" s="13"/>
@@ -2624,19 +2630,19 @@
       <c r="AC6" s="21"/>
       <c r="AD6" s="22"/>
     </row>
-    <row r="7" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" s="12" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="35">
+      <c r="D7" s="34">
         <v>1</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
@@ -2652,7 +2658,7 @@
       </c>
       <c r="M7" s="13"/>
       <c r="N7" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O7" s="18"/>
       <c r="P7" s="19">
@@ -2662,23 +2668,23 @@
       <c r="R7" s="18"/>
       <c r="S7" s="13"/>
       <c r="T7" s="20" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="U7" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="W7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="W7" s="13" t="s">
-        <v>9</v>
-      </c>
       <c r="X7" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Y7" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>serial1.line06.as1qa1.U.S</v>
+        <v>workorder1.line06.as1qa1.U.S</v>
       </c>
       <c r="Z7" s="13"/>
       <c r="AA7" s="13"/>
@@ -2686,19 +2692,19 @@
       <c r="AC7" s="21"/>
       <c r="AD7" s="22"/>
     </row>
-    <row r="8" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="35">
+      <c r="D8" s="34">
         <v>1</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
@@ -2714,7 +2720,7 @@
       </c>
       <c r="M8" s="13"/>
       <c r="N8" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O8" s="18"/>
       <c r="P8" s="19">
@@ -2724,23 +2730,23 @@
       <c r="R8" s="18"/>
       <c r="S8" s="13"/>
       <c r="T8" s="20" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="U8" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="W8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="W8" s="13" t="s">
-        <v>9</v>
-      </c>
       <c r="X8" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Y8" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>serial1.line07.as1qa1.U.S</v>
+        <v>workorder1.line07.as1qa1.U.S</v>
       </c>
       <c r="Z8" s="13"/>
       <c r="AA8" s="13"/>
@@ -2748,19 +2754,19 @@
       <c r="AC8" s="21"/>
       <c r="AD8" s="22"/>
     </row>
-    <row r="9" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="35">
+      <c r="D9" s="34">
         <v>1</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
@@ -2776,7 +2782,7 @@
       </c>
       <c r="M9" s="13"/>
       <c r="N9" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O9" s="18"/>
       <c r="P9" s="19">
@@ -2786,23 +2792,23 @@
       <c r="R9" s="18"/>
       <c r="S9" s="13"/>
       <c r="T9" s="20" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="U9" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="W9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="W9" s="13" t="s">
-        <v>9</v>
-      </c>
       <c r="X9" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Y9" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>serial1.line08.as1qa1.U.S</v>
+        <v>workorder1.line08.as1qa1.U.S</v>
       </c>
       <c r="Z9" s="13"/>
       <c r="AA9" s="13"/>
@@ -2810,19 +2816,19 @@
       <c r="AC9" s="21"/>
       <c r="AD9" s="22"/>
     </row>
-    <row r="10" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" s="12" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="35">
+      <c r="D10" s="34">
         <v>1</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
@@ -2838,7 +2844,7 @@
       </c>
       <c r="M10" s="13"/>
       <c r="N10" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O10" s="18"/>
       <c r="P10" s="19">
@@ -2848,23 +2854,23 @@
       <c r="R10" s="18"/>
       <c r="S10" s="13"/>
       <c r="T10" s="20" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="U10" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="W10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="W10" s="13" t="s">
+      <c r="X10" s="13" t="s">
         <v>9</v>
-      </c>
-      <c r="X10" s="13" t="s">
-        <v>10</v>
       </c>
       <c r="Y10" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>serial1.line09.as1qa1.S</v>
+        <v>workorder1.line09.as1qa1.S</v>
       </c>
       <c r="Z10" s="13"/>
       <c r="AA10" s="13"/>
@@ -2872,19 +2878,19 @@
       <c r="AC10" s="21"/>
       <c r="AD10" s="22"/>
     </row>
-    <row r="11" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" s="12" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="35">
+      <c r="D11" s="34">
         <v>1</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
@@ -2900,7 +2906,7 @@
       </c>
       <c r="M11" s="13"/>
       <c r="N11" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O11" s="18"/>
       <c r="P11" s="19">
@@ -2910,23 +2916,23 @@
       <c r="R11" s="18"/>
       <c r="S11" s="13"/>
       <c r="T11" s="20" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="U11" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="V11" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="W11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="W11" s="13" t="s">
+      <c r="X11" s="13" t="s">
         <v>9</v>
-      </c>
-      <c r="X11" s="13" t="s">
-        <v>10</v>
       </c>
       <c r="Y11" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>serial1.line10.as1qa1.S</v>
+        <v>workorder1.line10.as1qa1.S</v>
       </c>
       <c r="Z11" s="13"/>
       <c r="AA11" s="13"/>
@@ -2934,19 +2940,19 @@
       <c r="AC11" s="21"/>
       <c r="AD11" s="22"/>
     </row>
-    <row r="12" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="35">
+      <c r="D12" s="34">
         <v>1</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
@@ -2962,7 +2968,7 @@
       </c>
       <c r="M12" s="13"/>
       <c r="N12" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O12" s="18"/>
       <c r="P12" s="19">
@@ -2972,23 +2978,23 @@
       <c r="R12" s="18"/>
       <c r="S12" s="13"/>
       <c r="T12" s="20" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="U12" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="V12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="W12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="W12" s="13" t="s">
+      <c r="X12" s="13" t="s">
         <v>9</v>
-      </c>
-      <c r="X12" s="13" t="s">
-        <v>10</v>
       </c>
       <c r="Y12" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>serial1.line11.as1qa1.S</v>
+        <v>workorder1.line11.as1qa1.S</v>
       </c>
       <c r="Z12" s="13"/>
       <c r="AA12" s="13"/>
@@ -2996,19 +3002,19 @@
       <c r="AC12" s="21"/>
       <c r="AD12" s="22"/>
     </row>
-    <row r="13" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="35">
+      <c r="D13" s="34">
         <v>1</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
@@ -3024,7 +3030,7 @@
       </c>
       <c r="M13" s="13"/>
       <c r="N13" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O13" s="18"/>
       <c r="P13" s="19">
@@ -3034,23 +3040,23 @@
       <c r="R13" s="18"/>
       <c r="S13" s="13"/>
       <c r="T13" s="20" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="U13" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="V13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="W13" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="W13" s="13" t="s">
+      <c r="X13" s="13" t="s">
         <v>9</v>
-      </c>
-      <c r="X13" s="13" t="s">
-        <v>10</v>
       </c>
       <c r="Y13" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>serial1.line12.as1qa1.S</v>
+        <v>workorder1.line12.as1qa1.S</v>
       </c>
       <c r="Z13" s="13"/>
       <c r="AA13" s="13"/>
@@ -3058,7 +3064,7 @@
       <c r="AC13" s="21"/>
       <c r="AD13" s="22"/>
     </row>
-    <row r="14" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="23">
         <v>3854.12</v>
@@ -3066,54 +3072,54 @@
       <c r="C14" s="23">
         <v>14</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D14" s="35">
         <f>SUM(D2:D13)</f>
         <v>44</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H14" s="26"/>
       <c r="I14" s="26"/>
       <c r="J14" s="26"/>
-      <c r="K14" s="27">
-        <f>SUM(K2:K13)</f>
-        <v>420</v>
-      </c>
-      <c r="L14" s="28"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27">
+        <f>SUM(L2:L13)</f>
+        <v>770</v>
+      </c>
       <c r="M14" s="24"/>
-      <c r="N14" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="29"/>
+      <c r="N14" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
       <c r="S14" s="24"/>
-      <c r="T14" s="30"/>
+      <c r="T14" s="29"/>
       <c r="U14" s="24"/>
       <c r="V14" s="24"/>
       <c r="W14" s="24"/>
       <c r="X14" s="24"/>
-      <c r="Y14" s="40" t="str">
+      <c r="Y14" s="39" t="str">
         <f t="shared" si="0"/>
         <v>...</v>
       </c>
       <c r="Z14" s="24"/>
       <c r="AA14" s="24"/>
-      <c r="AB14" s="29"/>
-      <c r="AC14" s="29"/>
-      <c r="AD14" s="31"/>
+      <c r="AB14" s="28"/>
+      <c r="AC14" s="28"/>
+      <c r="AD14" s="30"/>
     </row>
-    <row r="15" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:30" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="34"/>
+      <c r="D15" s="33"/>
       <c r="E15" s="3"/>
       <c r="F15" s="4"/>
       <c r="G15" s="3"/>
@@ -3145,24 +3151,24 @@
       <c r="AC15" s="8"/>
       <c r="AD15" s="11"/>
     </row>
-    <row r="16" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" s="12" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="35">
+      <c r="D16" s="34">
         <v>1</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
       <c r="J16" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K16" s="16">
         <v>15</v>
@@ -3173,7 +3179,7 @@
       </c>
       <c r="M16" s="13"/>
       <c r="N16" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O16" s="18"/>
       <c r="P16" s="19">
@@ -3183,23 +3189,23 @@
       <c r="R16" s="18"/>
       <c r="S16" s="13"/>
       <c r="T16" s="20" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="U16" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="V16" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="V16" s="13" t="s">
+      <c r="W16" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="W16" s="13" t="s">
-        <v>9</v>
-      </c>
       <c r="X16" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Y16" s="13" t="str">
         <f>CONCATENATE(T16,".",U16,".",V16,W16,".",X16)</f>
-        <v>serial2.line01.as1qa1.U.S</v>
+        <v>workorder2.line01.as1qa1.U.S</v>
       </c>
       <c r="Z16" s="13"/>
       <c r="AA16" s="13"/>
@@ -3207,24 +3213,24 @@
       <c r="AC16" s="21"/>
       <c r="AD16" s="22"/>
     </row>
-    <row r="17" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="35">
+      <c r="D17" s="34">
         <v>1</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K17" s="16">
         <v>40</v>
@@ -3235,7 +3241,7 @@
       </c>
       <c r="M17" s="13"/>
       <c r="N17" s="18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O17" s="18"/>
       <c r="P17" s="19">
@@ -3243,27 +3249,27 @@
       </c>
       <c r="Q17" s="18"/>
       <c r="R17" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="S17" s="13"/>
       <c r="T17" s="20" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="U17" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="V17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="W17" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="X17" s="13" t="s">
         <v>15</v>
-      </c>
-      <c r="V17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="W17" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="X17" s="13" t="s">
-        <v>16</v>
       </c>
       <c r="Y17" s="13" t="str">
         <f>CONCATENATE(T17,".",U17,".",V17,W17,".",X17)</f>
-        <v>serial2.line02.as1qa1.U.S</v>
+        <v>workorder2.line02.as1qa1.U.S</v>
       </c>
       <c r="Z17" s="13"/>
       <c r="AA17" s="13"/>
@@ -3271,7 +3277,7 @@
       <c r="AC17" s="21"/>
       <c r="AD17" s="22"/>
     </row>
-    <row r="18" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:30" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
       <c r="B18" s="23">
         <v>582.34</v>
@@ -3279,54 +3285,54 @@
       <c r="C18" s="23">
         <v>2</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D18" s="35">
         <f>SUM(D16:D17)</f>
         <v>2</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F18" s="25"/>
       <c r="G18" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
       <c r="J18" s="26"/>
-      <c r="K18" s="27">
-        <f>SUM(K16:K17)</f>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27">
+        <f>SUM(L16:L17)</f>
         <v>55</v>
       </c>
-      <c r="L18" s="28"/>
       <c r="M18" s="24"/>
-      <c r="N18" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="O18" s="29"/>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="29"/>
-      <c r="R18" s="29"/>
+      <c r="N18" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
       <c r="S18" s="24"/>
-      <c r="T18" s="30"/>
+      <c r="T18" s="29"/>
       <c r="U18" s="24"/>
       <c r="V18" s="24"/>
       <c r="W18" s="24"/>
       <c r="X18" s="24"/>
-      <c r="Y18" s="40" t="str">
+      <c r="Y18" s="39" t="str">
         <f t="shared" ref="Y18" si="3">CONCATENATE(T18,".",U18,".",V18,W18,".",X18)</f>
         <v>...</v>
       </c>
       <c r="Z18" s="24"/>
       <c r="AA18" s="24"/>
-      <c r="AB18" s="29"/>
-      <c r="AC18" s="29"/>
-      <c r="AD18" s="31"/>
+      <c r="AB18" s="28"/>
+      <c r="AC18" s="28"/>
+      <c r="AD18" s="30"/>
     </row>
-    <row r="19" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:30" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="34"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="3"/>
       <c r="F19" s="4"/>
       <c r="G19" s="3"/>
@@ -3358,19 +3364,19 @@
       <c r="AC19" s="8"/>
       <c r="AD19" s="11"/>
     </row>
-    <row r="20" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="35">
+      <c r="D20" s="34">
         <v>2</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
@@ -3386,7 +3392,7 @@
       </c>
       <c r="M20" s="13"/>
       <c r="N20" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O20" s="18"/>
       <c r="P20" s="19">
@@ -3396,23 +3402,23 @@
       <c r="R20" s="18"/>
       <c r="S20" s="13"/>
       <c r="T20" s="20" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="U20" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="V20" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="V20" s="13" t="s">
+      <c r="W20" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="W20" s="13" t="s">
+      <c r="X20" s="13" t="s">
         <v>9</v>
-      </c>
-      <c r="X20" s="13" t="s">
-        <v>10</v>
       </c>
       <c r="Y20" s="13" t="str">
         <f>CONCATENATE(T20,".",U20,".",V20,W20,".",X20)</f>
-        <v>serial3.line01.as1qa1.S</v>
+        <v>workorder3.line01.as1qa1.S</v>
       </c>
       <c r="Z20" s="13"/>
       <c r="AA20" s="13"/>
@@ -3420,7 +3426,7 @@
       <c r="AC20" s="21"/>
       <c r="AD20" s="22"/>
     </row>
-    <row r="21" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:30" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
       <c r="B21" s="23">
         <v>646.96</v>
@@ -3428,54 +3434,54 @@
       <c r="C21" s="23">
         <v>2</v>
       </c>
-      <c r="D21" s="36">
+      <c r="D21" s="35">
         <f>SUM(D20:D20)</f>
         <v>2</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F21" s="25"/>
       <c r="G21" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H21" s="26"/>
       <c r="I21" s="26"/>
       <c r="J21" s="26"/>
-      <c r="K21" s="27">
-        <f>SUM(K20:K20)</f>
-        <v>50</v>
-      </c>
-      <c r="L21" s="28"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27">
+        <f>SUM(L20:L20)</f>
+        <v>100</v>
+      </c>
       <c r="M21" s="24"/>
-      <c r="N21" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="O21" s="29"/>
-      <c r="P21" s="29"/>
-      <c r="Q21" s="29"/>
-      <c r="R21" s="29"/>
+      <c r="N21" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="28"/>
       <c r="S21" s="24"/>
-      <c r="T21" s="30"/>
+      <c r="T21" s="29"/>
       <c r="U21" s="24"/>
       <c r="V21" s="24"/>
       <c r="W21" s="24"/>
       <c r="X21" s="24"/>
-      <c r="Y21" s="40" t="str">
+      <c r="Y21" s="39" t="str">
         <f t="shared" ref="Y21" si="5">CONCATENATE(T21,".",U21,".",V21,W21,".",X21)</f>
         <v>...</v>
       </c>
       <c r="Z21" s="24"/>
       <c r="AA21" s="24"/>
-      <c r="AB21" s="29"/>
-      <c r="AC21" s="29"/>
-      <c r="AD21" s="31"/>
+      <c r="AB21" s="28"/>
+      <c r="AC21" s="28"/>
+      <c r="AD21" s="30"/>
     </row>
-    <row r="22" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:30" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="34"/>
+      <c r="D22" s="33"/>
       <c r="E22" s="3"/>
       <c r="F22" s="4"/>
       <c r="G22" s="3"/>
@@ -3507,24 +3513,24 @@
       <c r="AC22" s="8"/>
       <c r="AD22" s="11"/>
     </row>
-    <row r="23" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="35">
+      <c r="D23" s="34">
         <v>4</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
       <c r="J23" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K23" s="16">
         <v>20</v>
@@ -3535,7 +3541,7 @@
       </c>
       <c r="M23" s="13"/>
       <c r="N23" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O23" s="18"/>
       <c r="P23" s="19">
@@ -3545,23 +3551,23 @@
       <c r="R23" s="18"/>
       <c r="S23" s="13"/>
       <c r="T23" s="20" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="U23" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="V23" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="V23" s="13" t="s">
+      <c r="W23" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="W23" s="13" t="s">
-        <v>9</v>
-      </c>
       <c r="X23" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Y23" s="13" t="str">
         <f>CONCATENATE(T23,".",U23,".",V23,W23,".",X23)</f>
-        <v>serial4.line01.as1qa1.U.S</v>
+        <v>workorder4.line01.as1qa1.U.S</v>
       </c>
       <c r="Z23" s="13"/>
       <c r="AA23" s="13"/>
@@ -3569,24 +3575,24 @@
       <c r="AC23" s="21"/>
       <c r="AD23" s="22"/>
     </row>
-    <row r="24" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="35">
+      <c r="D24" s="34">
         <v>1</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
       <c r="J24" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K24" s="16">
         <v>30</v>
@@ -3597,7 +3603,7 @@
       </c>
       <c r="M24" s="13"/>
       <c r="N24" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O24" s="18"/>
       <c r="P24" s="19">
@@ -3607,23 +3613,23 @@
       <c r="R24" s="18"/>
       <c r="S24" s="13"/>
       <c r="T24" s="20" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="U24" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="V24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="W24" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="X24" s="13" t="s">
         <v>15</v>
-      </c>
-      <c r="V24" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="W24" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="X24" s="13" t="s">
-        <v>16</v>
       </c>
       <c r="Y24" s="13" t="str">
         <f>CONCATENATE(T24,".",U24,".",V24,W24,".",X24)</f>
-        <v>serial4.line02.as1qa1.U.S</v>
+        <v>workorder4.line02.as1qa1.U.S</v>
       </c>
       <c r="Z24" s="13"/>
       <c r="AA24" s="13"/>
@@ -3631,24 +3637,24 @@
       <c r="AC24" s="21"/>
       <c r="AD24" s="22"/>
     </row>
-    <row r="25" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="35">
+      <c r="D25" s="34">
         <v>1</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
       <c r="J25" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K25" s="16">
         <v>50</v>
@@ -3659,7 +3665,7 @@
       </c>
       <c r="M25" s="13"/>
       <c r="N25" s="18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="O25" s="18"/>
       <c r="P25" s="19">
@@ -3667,27 +3673,27 @@
       </c>
       <c r="Q25" s="18"/>
       <c r="R25" s="18" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="S25" s="13"/>
       <c r="T25" s="20" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="U25" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="V25" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="W25" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="W25" s="13" t="s">
+      <c r="X25" s="13" t="s">
         <v>9</v>
-      </c>
-      <c r="X25" s="13" t="s">
-        <v>10</v>
       </c>
       <c r="Y25" s="13" t="str">
         <f>CONCATENATE(T25,".",U25,".",V25,W25,".",X25)</f>
-        <v>serial4.line03.as1qa1.S</v>
+        <v>workorder4.line03.as1qa1.S</v>
       </c>
       <c r="Z25" s="13"/>
       <c r="AA25" s="13"/>
@@ -3695,7 +3701,7 @@
       <c r="AC25" s="21"/>
       <c r="AD25" s="22"/>
     </row>
-    <row r="26" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:30" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
       <c r="B26" s="23">
         <v>1055.26</v>
@@ -3703,54 +3709,54 @@
       <c r="C26" s="23">
         <v>6</v>
       </c>
-      <c r="D26" s="36">
+      <c r="D26" s="35">
         <f>SUM(D23:D25)</f>
         <v>6</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F26" s="25"/>
       <c r="G26" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H26" s="26"/>
       <c r="I26" s="26"/>
       <c r="J26" s="26"/>
-      <c r="K26" s="27">
-        <f>SUM(K23:K25)</f>
-        <v>100</v>
-      </c>
-      <c r="L26" s="28"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27">
+        <f>SUM(L23:L25)</f>
+        <v>160</v>
+      </c>
       <c r="M26" s="24"/>
-      <c r="N26" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="O26" s="29"/>
-      <c r="P26" s="29"/>
-      <c r="Q26" s="29"/>
-      <c r="R26" s="29"/>
+      <c r="N26" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="O26" s="28"/>
+      <c r="P26" s="28"/>
+      <c r="Q26" s="28"/>
+      <c r="R26" s="28"/>
       <c r="S26" s="24"/>
-      <c r="T26" s="30"/>
+      <c r="T26" s="29"/>
       <c r="U26" s="24"/>
       <c r="V26" s="24"/>
       <c r="W26" s="24"/>
       <c r="X26" s="24"/>
-      <c r="Y26" s="40" t="str">
+      <c r="Y26" s="39" t="str">
         <f t="shared" ref="Y26" si="7">CONCATENATE(T26,".",U26,".",V26,W26,".",X26)</f>
         <v>...</v>
       </c>
       <c r="Z26" s="24"/>
       <c r="AA26" s="24"/>
-      <c r="AB26" s="29"/>
-      <c r="AC26" s="29"/>
-      <c r="AD26" s="31"/>
+      <c r="AB26" s="28"/>
+      <c r="AC26" s="28"/>
+      <c r="AD26" s="30"/>
     </row>
-    <row r="27" spans="1:30" s="12" customFormat="1" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:30" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="34"/>
+      <c r="D27" s="33"/>
       <c r="E27" s="3"/>
       <c r="F27" s="4"/>
       <c r="G27" s="3"/>
@@ -3782,115 +3788,115 @@
       <c r="AC27" s="8"/>
       <c r="AD27" s="11"/>
     </row>
-    <row r="28" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="36">
+      <c r="D28" s="35">
         <v>3</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F28" s="25"/>
       <c r="G28" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H28" s="26"/>
       <c r="I28" s="26"/>
-      <c r="J28" s="39" t="s">
-        <v>13</v>
+      <c r="J28" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="K28" s="27">
         <v>10</v>
       </c>
-      <c r="L28" s="38">
-        <f t="shared" ref="L28:L29" si="8">PRODUCT(D28, K28)</f>
+      <c r="L28" s="37">
+        <f t="shared" ref="L28:L32" si="8">PRODUCT(D28, K28)</f>
         <v>30</v>
       </c>
       <c r="M28" s="24"/>
-      <c r="N28" s="29" t="s">
+      <c r="N28" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="O28" s="29"/>
-      <c r="P28" s="32">
+      <c r="O28" s="28"/>
+      <c r="P28" s="31">
         <v>43451</v>
       </c>
-      <c r="Q28" s="29"/>
-      <c r="R28" s="29"/>
+      <c r="Q28" s="28"/>
+      <c r="R28" s="28"/>
       <c r="S28" s="24"/>
-      <c r="T28" s="30"/>
+      <c r="T28" s="29"/>
       <c r="U28" s="24"/>
       <c r="V28" s="24"/>
       <c r="W28" s="24"/>
       <c r="X28" s="24"/>
-      <c r="Y28" s="40" t="str">
+      <c r="Y28" s="39" t="str">
         <f t="shared" ref="Y28:Y32" si="9">CONCATENATE(T28,".",U28,".",V28,W28,".",X28)</f>
         <v>...</v>
       </c>
       <c r="Z28" s="24"/>
       <c r="AA28" s="24"/>
-      <c r="AB28" s="29"/>
-      <c r="AC28" s="33"/>
+      <c r="AB28" s="28"/>
+      <c r="AC28" s="32"/>
       <c r="AD28" s="22"/>
     </row>
-    <row r="29" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:30" s="12" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="36">
+      <c r="D29" s="35">
         <v>2</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F29" s="25"/>
       <c r="G29" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H29" s="26"/>
       <c r="I29" s="26"/>
       <c r="J29" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K29" s="27">
         <v>30</v>
       </c>
-      <c r="L29" s="38">
+      <c r="L29" s="37">
         <f t="shared" si="8"/>
         <v>60</v>
       </c>
       <c r="M29" s="24"/>
-      <c r="N29" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="O29" s="29"/>
-      <c r="P29" s="32">
+      <c r="N29" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="O29" s="28"/>
+      <c r="P29" s="31">
         <v>43451</v>
       </c>
-      <c r="Q29" s="29"/>
-      <c r="R29" s="29"/>
+      <c r="Q29" s="28"/>
+      <c r="R29" s="28"/>
       <c r="S29" s="24"/>
-      <c r="T29" s="30"/>
+      <c r="T29" s="29"/>
       <c r="U29" s="24"/>
       <c r="V29" s="24"/>
       <c r="W29" s="24"/>
       <c r="X29" s="24"/>
-      <c r="Y29" s="40" t="str">
+      <c r="Y29" s="39" t="str">
         <f t="shared" si="9"/>
         <v>...</v>
       </c>
       <c r="Z29" s="24"/>
       <c r="AA29" s="24"/>
-      <c r="AB29" s="29"/>
-      <c r="AC29" s="33"/>
+      <c r="AB29" s="28"/>
+      <c r="AC29" s="32"/>
       <c r="AD29" s="22"/>
     </row>
-    <row r="30" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="36"/>
+      <c r="D30" s="35"/>
       <c r="E30" s="24"/>
       <c r="F30" s="25"/>
       <c r="G30" s="24"/>
@@ -3898,34 +3904,37 @@
       <c r="I30" s="26"/>
       <c r="J30" s="26"/>
       <c r="K30" s="27"/>
-      <c r="L30" s="28"/>
+      <c r="L30" s="40">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="M30" s="24"/>
-      <c r="N30" s="29"/>
-      <c r="O30" s="29"/>
-      <c r="P30" s="32"/>
-      <c r="Q30" s="29"/>
-      <c r="R30" s="29"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="31"/>
+      <c r="Q30" s="28"/>
+      <c r="R30" s="28"/>
       <c r="S30" s="24"/>
-      <c r="T30" s="30"/>
+      <c r="T30" s="29"/>
       <c r="U30" s="24"/>
       <c r="V30" s="24"/>
       <c r="W30" s="24"/>
       <c r="X30" s="24"/>
-      <c r="Y30" s="40" t="str">
+      <c r="Y30" s="39" t="str">
         <f t="shared" si="9"/>
         <v>...</v>
       </c>
       <c r="Z30" s="24"/>
       <c r="AA30" s="24"/>
-      <c r="AB30" s="29"/>
-      <c r="AC30" s="33"/>
+      <c r="AB30" s="28"/>
+      <c r="AC30" s="32"/>
       <c r="AD30" s="22"/>
     </row>
-    <row r="31" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="36"/>
+      <c r="D31" s="35"/>
       <c r="E31" s="24"/>
       <c r="F31" s="25"/>
       <c r="G31" s="24"/>
@@ -3933,34 +3942,37 @@
       <c r="I31" s="26"/>
       <c r="J31" s="26"/>
       <c r="K31" s="27"/>
-      <c r="L31" s="28"/>
+      <c r="L31" s="40">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="M31" s="24"/>
-      <c r="N31" s="29"/>
-      <c r="O31" s="29"/>
-      <c r="P31" s="32"/>
-      <c r="Q31" s="29"/>
-      <c r="R31" s="29"/>
+      <c r="N31" s="28"/>
+      <c r="O31" s="28"/>
+      <c r="P31" s="31"/>
+      <c r="Q31" s="28"/>
+      <c r="R31" s="28"/>
       <c r="S31" s="24"/>
-      <c r="T31" s="30"/>
+      <c r="T31" s="29"/>
       <c r="U31" s="24"/>
       <c r="V31" s="24"/>
       <c r="W31" s="24"/>
       <c r="X31" s="24"/>
-      <c r="Y31" s="40" t="str">
+      <c r="Y31" s="39" t="str">
         <f t="shared" si="9"/>
         <v>...</v>
       </c>
       <c r="Z31" s="24"/>
       <c r="AA31" s="24"/>
-      <c r="AB31" s="29"/>
-      <c r="AC31" s="33"/>
+      <c r="AB31" s="28"/>
+      <c r="AC31" s="32"/>
       <c r="AD31" s="22"/>
     </row>
-    <row r="32" spans="1:30" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:30" s="12" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="36"/>
+      <c r="D32" s="35"/>
       <c r="E32" s="24"/>
       <c r="F32" s="25"/>
       <c r="G32" s="24"/>
@@ -3968,27 +3980,30 @@
       <c r="I32" s="26"/>
       <c r="J32" s="26"/>
       <c r="K32" s="27"/>
-      <c r="L32" s="28"/>
+      <c r="L32" s="40">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="M32" s="24"/>
-      <c r="N32" s="29"/>
-      <c r="O32" s="29"/>
-      <c r="P32" s="32"/>
-      <c r="Q32" s="29"/>
-      <c r="R32" s="29"/>
+      <c r="N32" s="28"/>
+      <c r="O32" s="28"/>
+      <c r="P32" s="31"/>
+      <c r="Q32" s="28"/>
+      <c r="R32" s="28"/>
       <c r="S32" s="24"/>
-      <c r="T32" s="30"/>
+      <c r="T32" s="29"/>
       <c r="U32" s="24"/>
       <c r="V32" s="24"/>
       <c r="W32" s="24"/>
       <c r="X32" s="24"/>
-      <c r="Y32" s="40" t="str">
+      <c r="Y32" s="39" t="str">
         <f t="shared" si="9"/>
         <v>...</v>
       </c>
       <c r="Z32" s="24"/>
       <c r="AA32" s="24"/>
-      <c r="AB32" s="29"/>
-      <c r="AC32" s="33"/>
+      <c r="AB32" s="28"/>
+      <c r="AC32" s="32"/>
       <c r="AD32" s="22"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get all rows which have a cylinder and not a workorder number
</commit_message>
<xml_diff>
--- a/data/Scrubbed Data.xlsx
+++ b/data/Scrubbed Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guysbryant/code/Personal/learn_ruby_spreadsheets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8416775-2DDE-774C-A780-662E472C0EBE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B3D234-7B9B-E745-B3C4-627B3FA19059}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="68">
   <si>
     <t>MODEL</t>
   </si>
@@ -372,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -476,11 +476,150 @@
     <xf numFmtId="4" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="138">
+  <dxfs count="150">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2262,10 +2401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD32"/>
+  <dimension ref="A1:AD34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3811,7 +3950,7 @@
         <v>10</v>
       </c>
       <c r="L28" s="37">
-        <f t="shared" ref="L28:L32" si="8">PRODUCT(D28, K28)</f>
+        <f t="shared" ref="L28:L34" si="8">PRODUCT(D28, K28)</f>
         <v>30</v>
       </c>
       <c r="M28" s="24"/>
@@ -3820,7 +3959,7 @@
       </c>
       <c r="O28" s="28"/>
       <c r="P28" s="31">
-        <v>43451</v>
+        <v>43482</v>
       </c>
       <c r="Q28" s="28"/>
       <c r="R28" s="28"/>
@@ -3831,7 +3970,7 @@
       <c r="W28" s="24"/>
       <c r="X28" s="24"/>
       <c r="Y28" s="39" t="str">
-        <f t="shared" ref="Y28:Y32" si="9">CONCATENATE(T28,".",U28,".",V28,W28,".",X28)</f>
+        <f t="shared" ref="Y28:Y34" si="9">CONCATENATE(T28,".",U28,".",V28,W28,".",X28)</f>
         <v>...</v>
       </c>
       <c r="Z28" s="24"/>
@@ -3872,7 +4011,7 @@
       </c>
       <c r="O29" s="28"/>
       <c r="P29" s="31">
-        <v>43451</v>
+        <v>43237</v>
       </c>
       <c r="Q29" s="28"/>
       <c r="R29" s="28"/>
@@ -3896,79 +4035,101 @@
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="40">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="M30" s="24"/>
-      <c r="N30" s="28"/>
-      <c r="O30" s="28"/>
-      <c r="P30" s="31"/>
-      <c r="Q30" s="28"/>
-      <c r="R30" s="28"/>
-      <c r="S30" s="24"/>
-      <c r="T30" s="29"/>
-      <c r="U30" s="24"/>
-      <c r="V30" s="24"/>
-      <c r="W30" s="24"/>
-      <c r="X30" s="24"/>
-      <c r="Y30" s="39" t="str">
-        <f t="shared" si="9"/>
-        <v>...</v>
-      </c>
-      <c r="Z30" s="24"/>
-      <c r="AA30" s="24"/>
-      <c r="AB30" s="28"/>
-      <c r="AC30" s="32"/>
+      <c r="D30" s="41">
+        <v>30</v>
+      </c>
+      <c r="E30" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="42"/>
+      <c r="G30" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="K30" s="43">
+        <v>10</v>
+      </c>
+      <c r="L30" s="37">
+        <f>PRODUCT(D30, K30)</f>
+        <v>300</v>
+      </c>
+      <c r="M30" s="39"/>
+      <c r="N30" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="O30" s="44"/>
+      <c r="P30" s="45">
+        <v>43448</v>
+      </c>
+      <c r="Q30" s="44"/>
+      <c r="R30" s="44"/>
+      <c r="S30" s="39"/>
+      <c r="T30" s="46"/>
+      <c r="U30" s="39"/>
+      <c r="V30" s="39"/>
+      <c r="W30" s="39"/>
+      <c r="X30" s="39"/>
+      <c r="Y30" s="39"/>
+      <c r="Z30" s="39"/>
+      <c r="AA30" s="39"/>
+      <c r="AB30" s="44"/>
+      <c r="AC30" s="47"/>
       <c r="AD30" s="22"/>
     </row>
     <row r="31" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="40">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="M31" s="24"/>
-      <c r="N31" s="28"/>
-      <c r="O31" s="28"/>
-      <c r="P31" s="31"/>
-      <c r="Q31" s="28"/>
-      <c r="R31" s="28"/>
-      <c r="S31" s="24"/>
-      <c r="T31" s="29"/>
-      <c r="U31" s="24"/>
-      <c r="V31" s="24"/>
-      <c r="W31" s="24"/>
-      <c r="X31" s="24"/>
-      <c r="Y31" s="39" t="str">
-        <f t="shared" si="9"/>
-        <v>...</v>
-      </c>
-      <c r="Z31" s="24"/>
-      <c r="AA31" s="24"/>
-      <c r="AB31" s="28"/>
-      <c r="AC31" s="32"/>
+      <c r="D31" s="41">
+        <v>4</v>
+      </c>
+      <c r="E31" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="42"/>
+      <c r="G31" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="K31" s="43">
+        <v>20</v>
+      </c>
+      <c r="L31" s="37">
+        <f t="shared" ref="L31" si="10">PRODUCT(D31, K31)</f>
+        <v>80</v>
+      </c>
+      <c r="M31" s="39"/>
+      <c r="N31" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="O31" s="44"/>
+      <c r="P31" s="45">
+        <v>43439</v>
+      </c>
+      <c r="Q31" s="44"/>
+      <c r="R31" s="44"/>
+      <c r="S31" s="39"/>
+      <c r="T31" s="46"/>
+      <c r="U31" s="39"/>
+      <c r="V31" s="39"/>
+      <c r="W31" s="39"/>
+      <c r="X31" s="39"/>
+      <c r="Y31" s="39"/>
+      <c r="Z31" s="39"/>
+      <c r="AA31" s="39"/>
+      <c r="AB31" s="44"/>
+      <c r="AC31" s="47"/>
       <c r="AD31" s="22"/>
     </row>
-    <row r="32" spans="1:30" s="12" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -4006,510 +4167,630 @@
       <c r="AC32" s="32"/>
       <c r="AD32" s="22"/>
     </row>
+    <row r="33" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="1"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="27"/>
+      <c r="L33" s="40">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="24"/>
+      <c r="N33" s="28"/>
+      <c r="O33" s="28"/>
+      <c r="P33" s="31"/>
+      <c r="Q33" s="28"/>
+      <c r="R33" s="28"/>
+      <c r="S33" s="24"/>
+      <c r="T33" s="29"/>
+      <c r="U33" s="24"/>
+      <c r="V33" s="24"/>
+      <c r="W33" s="24"/>
+      <c r="X33" s="24"/>
+      <c r="Y33" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v>...</v>
+      </c>
+      <c r="Z33" s="24"/>
+      <c r="AA33" s="24"/>
+      <c r="AB33" s="28"/>
+      <c r="AC33" s="32"/>
+      <c r="AD33" s="22"/>
+    </row>
+    <row r="34" spans="1:30" s="12" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="1"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="40">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M34" s="24"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="28"/>
+      <c r="P34" s="31"/>
+      <c r="Q34" s="28"/>
+      <c r="R34" s="28"/>
+      <c r="S34" s="24"/>
+      <c r="T34" s="29"/>
+      <c r="U34" s="24"/>
+      <c r="V34" s="24"/>
+      <c r="W34" s="24"/>
+      <c r="X34" s="24"/>
+      <c r="Y34" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v>...</v>
+      </c>
+      <c r="Z34" s="24"/>
+      <c r="AA34" s="24"/>
+      <c r="AB34" s="28"/>
+      <c r="AC34" s="32"/>
+      <c r="AD34" s="22"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="P2">
-    <cfRule type="timePeriod" dxfId="137" priority="2" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="149" priority="14" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P2,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P2,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="136" priority="3" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="148" priority="15" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P2,1)&lt;=6,FLOOR(P2,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="135" priority="4" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="147" priority="16" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P2,1)&lt;=6,FLOOR(P2,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2">
-    <cfRule type="timePeriod" dxfId="134" priority="5" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="146" priority="17" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P2,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P2,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="133" priority="6" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="145" priority="18" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P2,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P2,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="132" priority="7" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="144" priority="19" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P2,1)&lt;=6,FLOOR(P2,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="timePeriod" dxfId="131" priority="8" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="143" priority="20" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P5,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P5,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="130" priority="9" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="142" priority="21" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P5,1)&lt;=6,FLOOR(P5,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="129" priority="10" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="141" priority="22" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P5,1)&lt;=6,FLOOR(P5,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="timePeriod" dxfId="128" priority="11" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="140" priority="23" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P5,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P5,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="127" priority="12" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="139" priority="24" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P5,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P5,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="126" priority="13" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="138" priority="25" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P5,1)&lt;=6,FLOOR(P5,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4">
-    <cfRule type="timePeriod" dxfId="125" priority="14" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="137" priority="26" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P4,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P4,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="124" priority="15" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="136" priority="27" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P4,1)&lt;=6,FLOOR(P4,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="123" priority="16" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="135" priority="28" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P4,1)&lt;=6,FLOOR(P4,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4">
-    <cfRule type="timePeriod" dxfId="122" priority="17" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="134" priority="29" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P4,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P4,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="121" priority="18" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="133" priority="30" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P4,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P4,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="120" priority="19" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="132" priority="31" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P4,1)&lt;=6,FLOOR(P4,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3">
-    <cfRule type="timePeriod" dxfId="119" priority="20" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="131" priority="32" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P3,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P3,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="118" priority="21" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="130" priority="33" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P3,1)&lt;=6,FLOOR(P3,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="117" priority="22" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="129" priority="34" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P3,1)&lt;=6,FLOOR(P3,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3">
-    <cfRule type="timePeriod" dxfId="116" priority="23" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="128" priority="35" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P3,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P3,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="115" priority="24" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="127" priority="36" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P3,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P3,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="114" priority="25" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="126" priority="37" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P3,1)&lt;=6,FLOOR(P3,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P7">
-    <cfRule type="timePeriod" dxfId="113" priority="26" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="125" priority="38" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P7,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P7,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="112" priority="27" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="124" priority="39" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P7,1)&lt;=6,FLOOR(P7,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="111" priority="28" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="123" priority="40" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P7,1)&lt;=6,FLOOR(P7,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P7">
-    <cfRule type="timePeriod" dxfId="110" priority="29" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="122" priority="41" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P7,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P7,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="109" priority="30" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="121" priority="42" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P7,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P7,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="108" priority="31" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="120" priority="43" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P7,1)&lt;=6,FLOOR(P7,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P6">
-    <cfRule type="timePeriod" dxfId="107" priority="32" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="119" priority="44" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P6,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P6,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="106" priority="33" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="118" priority="45" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P6,1)&lt;=6,FLOOR(P6,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="105" priority="34" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="117" priority="46" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P6,1)&lt;=6,FLOOR(P6,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P6">
-    <cfRule type="timePeriod" dxfId="104" priority="35" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="116" priority="47" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P6,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P6,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="103" priority="36" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="115" priority="48" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P6,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P6,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="102" priority="37" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="114" priority="49" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P6,1)&lt;=6,FLOOR(P6,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P8">
-    <cfRule type="timePeriod" dxfId="101" priority="38" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="113" priority="50" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P8,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P8,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="100" priority="39" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="112" priority="51" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P8,1)&lt;=6,FLOOR(P8,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="99" priority="40" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="111" priority="52" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P8,1)&lt;=6,FLOOR(P8,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P8">
-    <cfRule type="timePeriod" dxfId="98" priority="41" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="110" priority="53" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P8,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P8,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="97" priority="42" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="109" priority="54" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P8,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P8,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="96" priority="43" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="108" priority="55" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P8,1)&lt;=6,FLOOR(P8,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P10">
-    <cfRule type="timePeriod" dxfId="95" priority="44" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="107" priority="56" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P10,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P10,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="94" priority="45" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="106" priority="57" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P10,1)&lt;=6,FLOOR(P10,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="93" priority="46" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="105" priority="58" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P10,1)&lt;=6,FLOOR(P10,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P10">
-    <cfRule type="timePeriod" dxfId="92" priority="47" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="104" priority="59" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P10,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P10,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="91" priority="48" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="103" priority="60" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P10,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P10,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="90" priority="49" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="102" priority="61" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P10,1)&lt;=6,FLOOR(P10,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P9">
-    <cfRule type="timePeriod" dxfId="89" priority="50" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="101" priority="62" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P9,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P9,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="88" priority="51" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="100" priority="63" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P9,1)&lt;=6,FLOOR(P9,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="87" priority="52" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="99" priority="64" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P9,1)&lt;=6,FLOOR(P9,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P9">
-    <cfRule type="timePeriod" dxfId="86" priority="53" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="98" priority="65" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P9,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P9,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="85" priority="54" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="97" priority="66" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P9,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P9,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="84" priority="55" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="96" priority="67" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P9,1)&lt;=6,FLOOR(P9,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P12">
-    <cfRule type="timePeriod" dxfId="83" priority="56" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="95" priority="68" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P12,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P12,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="82" priority="57" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="94" priority="69" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P12,1)&lt;=6,FLOOR(P12,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="81" priority="58" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="93" priority="70" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P12,1)&lt;=6,FLOOR(P12,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P12">
-    <cfRule type="timePeriod" dxfId="80" priority="59" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="92" priority="71" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P12,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P12,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="79" priority="60" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="91" priority="72" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P12,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P12,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="78" priority="61" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="90" priority="73" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P12,1)&lt;=6,FLOOR(P12,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P11">
-    <cfRule type="timePeriod" dxfId="77" priority="62" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="89" priority="74" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P11,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P11,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="76" priority="63" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="88" priority="75" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P11,1)&lt;=6,FLOOR(P11,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="75" priority="64" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="87" priority="76" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P11,1)&lt;=6,FLOOR(P11,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P11">
-    <cfRule type="timePeriod" dxfId="74" priority="65" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="86" priority="77" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P11,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P11,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="73" priority="66" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="85" priority="78" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P11,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P11,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="72" priority="67" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="84" priority="79" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P11,1)&lt;=6,FLOOR(P11,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P24">
-    <cfRule type="timePeriod" dxfId="71" priority="68" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="83" priority="80" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P24,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P24,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="70" priority="69" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="82" priority="81" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P24,1)&lt;=6,FLOOR(P24,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="69" priority="70" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="81" priority="82" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P24,1)&lt;=6,FLOOR(P24,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P24">
-    <cfRule type="timePeriod" dxfId="68" priority="71" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="80" priority="83" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P24,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P24,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="67" priority="72" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="79" priority="84" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P24,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P24,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="66" priority="73" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="78" priority="85" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P24,1)&lt;=6,FLOOR(P24,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16">
-    <cfRule type="timePeriod" dxfId="65" priority="74" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="77" priority="86" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="64" priority="75" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="76" priority="87" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P16,1)&lt;=6,FLOOR(P16,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="63" priority="76" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="75" priority="88" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P16,1)&lt;=6,FLOOR(P16,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16">
-    <cfRule type="timePeriod" dxfId="62" priority="77" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="74" priority="89" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P16,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P16,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="61" priority="78" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="73" priority="90" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="60" priority="79" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="72" priority="91" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P16,1)&lt;=6,FLOOR(P16,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P13">
-    <cfRule type="timePeriod" dxfId="59" priority="80" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="71" priority="92" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P13,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P13,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="58" priority="81" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="70" priority="93" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P13,1)&lt;=6,FLOOR(P13,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="57" priority="82" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="69" priority="94" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P13,1)&lt;=6,FLOOR(P13,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P13">
-    <cfRule type="timePeriod" dxfId="56" priority="83" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="68" priority="95" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P13,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P13,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="55" priority="84" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="67" priority="96" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P13,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P13,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="54" priority="85" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="66" priority="97" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P13,1)&lt;=6,FLOOR(P13,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17">
-    <cfRule type="timePeriod" dxfId="53" priority="86" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="65" priority="98" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P17,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P17,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="52" priority="87" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="64" priority="99" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P17,1)&lt;=6,FLOOR(P17,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="51" priority="88" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="63" priority="100" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P17,1)&lt;=6,FLOOR(P17,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17">
-    <cfRule type="timePeriod" dxfId="50" priority="89" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="62" priority="101" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P17,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P17,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="49" priority="90" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="61" priority="102" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P17,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P17,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="48" priority="91" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="60" priority="103" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P17,1)&lt;=6,FLOOR(P17,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P20">
-    <cfRule type="timePeriod" dxfId="47" priority="92" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="59" priority="104" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P20,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P20,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="46" priority="93" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="58" priority="105" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P20,1)&lt;=6,FLOOR(P20,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="45" priority="94" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="57" priority="106" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P20,1)&lt;=6,FLOOR(P20,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P20">
-    <cfRule type="timePeriod" dxfId="44" priority="95" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="56" priority="107" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P20,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P20,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="43" priority="96" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="55" priority="108" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P20,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P20,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="42" priority="97" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="54" priority="109" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P20,1)&lt;=6,FLOOR(P20,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P23">
-    <cfRule type="timePeriod" dxfId="41" priority="98" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="53" priority="110" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P23,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P23,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="40" priority="99" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="52" priority="111" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P23,1)&lt;=6,FLOOR(P23,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="39" priority="100" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="51" priority="112" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P23,1)&lt;=6,FLOOR(P23,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P23">
-    <cfRule type="timePeriod" dxfId="38" priority="101" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="50" priority="113" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P23,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P23,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="37" priority="102" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="49" priority="114" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P23,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P23,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="36" priority="103" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="48" priority="115" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P23,1)&lt;=6,FLOOR(P23,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P25">
-    <cfRule type="timePeriod" dxfId="35" priority="104" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="47" priority="116" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P25,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P25,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="34" priority="105" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="46" priority="117" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P25,1)&lt;=6,FLOOR(P25,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="33" priority="106" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="45" priority="118" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P25,1)&lt;=6,FLOOR(P25,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P25">
-    <cfRule type="timePeriod" dxfId="32" priority="107" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="44" priority="119" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P25,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P25,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="31" priority="108" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="43" priority="120" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P25,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P25,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="30" priority="109" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="42" priority="121" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P25,1)&lt;=6,FLOOR(P25,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="P32">
+    <cfRule type="timePeriod" dxfId="41" priority="122" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P32,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P32,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="40" priority="123" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P32,1)&lt;=6,FLOOR(P32,1)&lt;=TODAY())</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="39" priority="124" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P32,1)&lt;=6,FLOOR(P32,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P32">
+    <cfRule type="timePeriod" dxfId="38" priority="125" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(P32,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P32,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="37" priority="126" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P32,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P32,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="36" priority="127" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P32,1)&lt;=6,FLOOR(P32,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P29">
+    <cfRule type="timePeriod" dxfId="35" priority="128" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P29,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P29,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="34" priority="129" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P29,1)&lt;=6,FLOOR(P29,1)&lt;=TODAY())</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="33" priority="130" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P29,1)&lt;=6,FLOOR(P29,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P29">
+    <cfRule type="timePeriod" dxfId="32" priority="131" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(P29,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P29,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="31" priority="132" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P29,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P29,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="30" priority="133" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P29,1)&lt;=6,FLOOR(P29,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P28">
+    <cfRule type="timePeriod" dxfId="29" priority="134" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P28,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P28,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="28" priority="135" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P28,1)&lt;=6,FLOOR(P28,1)&lt;=TODAY())</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="27" priority="136" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P28,1)&lt;=6,FLOOR(P28,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P28">
+    <cfRule type="timePeriod" dxfId="26" priority="137" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(P28,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P28,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="25" priority="138" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P28,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P28,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="24" priority="139" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P28,1)&lt;=6,FLOOR(P28,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P34">
+    <cfRule type="timePeriod" dxfId="23" priority="140" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P34,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P34,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="22" priority="141" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P34,1)&lt;=6,FLOOR(P34,1)&lt;=TODAY())</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="21" priority="142" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P34,1)&lt;=6,FLOOR(P34,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P34">
+    <cfRule type="timePeriod" dxfId="20" priority="143" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(P34,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P34,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="19" priority="144" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P34,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P34,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="18" priority="145" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P34,1)&lt;=6,FLOOR(P34,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P33">
+    <cfRule type="timePeriod" dxfId="17" priority="146" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P33,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P33,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="16" priority="147" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P33,1)&lt;=6,FLOOR(P33,1)&lt;=TODAY())</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="15" priority="148" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P33,1)&lt;=6,FLOOR(P33,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P33">
+    <cfRule type="timePeriod" dxfId="14" priority="149" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(P33,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P33,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="13" priority="150" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P33,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P33,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="12" priority="151" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P33,1)&lt;=6,FLOOR(P33,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="P30">
-    <cfRule type="timePeriod" dxfId="29" priority="110" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="11" priority="1" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P30,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P30,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="28" priority="111" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="10" priority="2" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P30,1)&lt;=6,FLOOR(P30,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="27" priority="112" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="9" priority="3" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P30,1)&lt;=6,FLOOR(P30,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P30">
-    <cfRule type="timePeriod" dxfId="26" priority="113" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="8" priority="4" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P30,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P30,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="25" priority="114" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="7" priority="5" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P30,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P30,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="24" priority="115" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="6" priority="6" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P30,1)&lt;=6,FLOOR(P30,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P29">
-    <cfRule type="timePeriod" dxfId="23" priority="116" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(P29,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P29,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="22" priority="117" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P29,1)&lt;=6,FLOOR(P29,1)&lt;=TODAY())</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="21" priority="118" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P29,1)&lt;=6,FLOOR(P29,1)&lt;=TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P29">
-    <cfRule type="timePeriod" dxfId="20" priority="119" timePeriod="thisWeek">
-      <formula>AND(TODAY()-ROUNDDOWN(P29,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P29,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="19" priority="120" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(P29,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P29,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="18" priority="121" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P29,1)&lt;=6,FLOOR(P29,1)&lt;=TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P28">
-    <cfRule type="timePeriod" dxfId="17" priority="122" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(P28,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P28,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="16" priority="123" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P28,1)&lt;=6,FLOOR(P28,1)&lt;=TODAY())</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="15" priority="124" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P28,1)&lt;=6,FLOOR(P28,1)&lt;=TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P28">
-    <cfRule type="timePeriod" dxfId="14" priority="125" timePeriod="thisWeek">
-      <formula>AND(TODAY()-ROUNDDOWN(P28,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P28,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="13" priority="126" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(P28,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P28,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="12" priority="127" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P28,1)&lt;=6,FLOOR(P28,1)&lt;=TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P32">
-    <cfRule type="timePeriod" dxfId="11" priority="128" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(P32,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P32,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="10" priority="129" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P32,1)&lt;=6,FLOOR(P32,1)&lt;=TODAY())</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="9" priority="130" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P32,1)&lt;=6,FLOOR(P32,1)&lt;=TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P32">
-    <cfRule type="timePeriod" dxfId="8" priority="131" timePeriod="thisWeek">
-      <formula>AND(TODAY()-ROUNDDOWN(P32,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P32,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="7" priority="132" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(P32,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P32,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="6" priority="133" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P32,1)&lt;=6,FLOOR(P32,1)&lt;=TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="P31">
-    <cfRule type="timePeriod" dxfId="5" priority="134" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="5" priority="7" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P31,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P31,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="4" priority="135" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="4" priority="8" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P31,1)&lt;=6,FLOOR(P31,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="3" priority="136" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="3" priority="9" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P31,1)&lt;=6,FLOOR(P31,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P31">
-    <cfRule type="timePeriod" dxfId="2" priority="137" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="2" priority="10" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P31,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P31,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="1" priority="138" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="1" priority="11" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P31,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P31,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="0" priority="139" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="0" priority="12" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P31,1)&lt;=6,FLOOR(P31,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
I don't really know what I've done because it has been so long since I looked at this
</commit_message>
<xml_diff>
--- a/data/Scrubbed Data.xlsx
+++ b/data/Scrubbed Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guysbryant/code/Personal/learn_ruby_spreadsheets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B3D234-7B9B-E745-B3C4-627B3FA19059}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E00C66F-9989-0A48-96DF-95352B0421E2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="69">
   <si>
     <t>MODEL</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>workorder4</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -277,7 +280,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,12 +296,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC5E0B4"/>
-        <bgColor rgb="FFCCFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
@@ -372,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -473,9 +470,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -499,67 +493,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="150">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="144">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2401,10 +2335,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD34"/>
+  <dimension ref="A1:AD33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3504,7 +3438,9 @@
       <c r="AD19" s="11"/>
     </row>
     <row r="20" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="34">
@@ -3950,7 +3886,7 @@
         <v>10</v>
       </c>
       <c r="L28" s="37">
-        <f t="shared" ref="L28:L34" si="8">PRODUCT(D28, K28)</f>
+        <f t="shared" ref="L28:L33" si="8">PRODUCT(D28, K28)</f>
         <v>30</v>
       </c>
       <c r="M28" s="24"/>
@@ -3970,7 +3906,7 @@
       <c r="W28" s="24"/>
       <c r="X28" s="24"/>
       <c r="Y28" s="39" t="str">
-        <f t="shared" ref="Y28:Y34" si="9">CONCATENATE(T28,".",U28,".",V28,W28,".",X28)</f>
+        <f t="shared" ref="Y28:Y33" si="9">CONCATENATE(T28,".",U28,".",V28,W28,".",X28)</f>
         <v>...</v>
       </c>
       <c r="Z28" s="24"/>
@@ -4035,13 +3971,13 @@
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="41">
+      <c r="D30" s="40">
         <v>30</v>
       </c>
       <c r="E30" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F30" s="42"/>
+      <c r="F30" s="41"/>
       <c r="G30" s="39" t="s">
         <v>3</v>
       </c>
@@ -4050,47 +3986,50 @@
       <c r="J30" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="K30" s="43">
+      <c r="K30" s="42">
         <v>10</v>
       </c>
       <c r="L30" s="37">
-        <f>PRODUCT(D30, K30)</f>
+        <f t="shared" si="8"/>
         <v>300</v>
       </c>
       <c r="M30" s="39"/>
-      <c r="N30" s="44" t="s">
+      <c r="N30" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="O30" s="44"/>
-      <c r="P30" s="45">
+      <c r="O30" s="43"/>
+      <c r="P30" s="44">
         <v>43448</v>
       </c>
-      <c r="Q30" s="44"/>
-      <c r="R30" s="44"/>
+      <c r="Q30" s="43"/>
+      <c r="R30" s="43"/>
       <c r="S30" s="39"/>
-      <c r="T30" s="46"/>
+      <c r="T30" s="45"/>
       <c r="U30" s="39"/>
       <c r="V30" s="39"/>
       <c r="W30" s="39"/>
       <c r="X30" s="39"/>
-      <c r="Y30" s="39"/>
+      <c r="Y30" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v>...</v>
+      </c>
       <c r="Z30" s="39"/>
       <c r="AA30" s="39"/>
-      <c r="AB30" s="44"/>
-      <c r="AC30" s="47"/>
+      <c r="AB30" s="43"/>
+      <c r="AC30" s="46"/>
       <c r="AD30" s="22"/>
     </row>
     <row r="31" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="41">
+      <c r="D31" s="40">
         <v>4</v>
       </c>
       <c r="E31" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="42"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="39" t="s">
         <v>11</v>
       </c>
@@ -4099,37 +4038,40 @@
       <c r="J31" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="K31" s="43">
+      <c r="K31" s="42">
         <v>20</v>
       </c>
       <c r="L31" s="37">
-        <f t="shared" ref="L31" si="10">PRODUCT(D31, K31)</f>
+        <f t="shared" si="8"/>
         <v>80</v>
       </c>
       <c r="M31" s="39"/>
-      <c r="N31" s="44" t="s">
+      <c r="N31" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="O31" s="44"/>
-      <c r="P31" s="45">
+      <c r="O31" s="43"/>
+      <c r="P31" s="44">
         <v>43439</v>
       </c>
-      <c r="Q31" s="44"/>
-      <c r="R31" s="44"/>
+      <c r="Q31" s="43"/>
+      <c r="R31" s="43"/>
       <c r="S31" s="39"/>
-      <c r="T31" s="46"/>
+      <c r="T31" s="45"/>
       <c r="U31" s="39"/>
       <c r="V31" s="39"/>
       <c r="W31" s="39"/>
       <c r="X31" s="39"/>
-      <c r="Y31" s="39"/>
+      <c r="Y31" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v>...</v>
+      </c>
       <c r="Z31" s="39"/>
       <c r="AA31" s="39"/>
-      <c r="AB31" s="44"/>
-      <c r="AC31" s="47"/>
+      <c r="AB31" s="43"/>
+      <c r="AC31" s="46"/>
       <c r="AD31" s="22"/>
     </row>
-    <row r="32" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:30" s="12" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -4141,7 +4083,7 @@
       <c r="I32" s="26"/>
       <c r="J32" s="26"/>
       <c r="K32" s="27"/>
-      <c r="L32" s="40">
+      <c r="L32" s="37">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4167,7 +4109,7 @@
       <c r="AC32" s="32"/>
       <c r="AD32" s="22"/>
     </row>
-    <row r="33" spans="1:30" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:30" s="12" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -4179,7 +4121,7 @@
       <c r="I33" s="26"/>
       <c r="J33" s="26"/>
       <c r="K33" s="27"/>
-      <c r="L33" s="40">
+      <c r="L33" s="37">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4205,593 +4147,533 @@
       <c r="AC33" s="32"/>
       <c r="AD33" s="22"/>
     </row>
-    <row r="34" spans="1:30" s="12" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="27"/>
-      <c r="L34" s="40">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="M34" s="24"/>
-      <c r="N34" s="28"/>
-      <c r="O34" s="28"/>
-      <c r="P34" s="31"/>
-      <c r="Q34" s="28"/>
-      <c r="R34" s="28"/>
-      <c r="S34" s="24"/>
-      <c r="T34" s="29"/>
-      <c r="U34" s="24"/>
-      <c r="V34" s="24"/>
-      <c r="W34" s="24"/>
-      <c r="X34" s="24"/>
-      <c r="Y34" s="39" t="str">
-        <f t="shared" si="9"/>
-        <v>...</v>
-      </c>
-      <c r="Z34" s="24"/>
-      <c r="AA34" s="24"/>
-      <c r="AB34" s="28"/>
-      <c r="AC34" s="32"/>
-      <c r="AD34" s="22"/>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="P2">
-    <cfRule type="timePeriod" dxfId="149" priority="14" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="143" priority="20" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P2,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P2,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="148" priority="15" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="142" priority="21" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P2,1)&lt;=6,FLOOR(P2,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="147" priority="16" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="141" priority="22" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P2,1)&lt;=6,FLOOR(P2,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2">
-    <cfRule type="timePeriod" dxfId="146" priority="17" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="140" priority="23" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P2,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P2,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="145" priority="18" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="139" priority="24" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P2,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P2,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="144" priority="19" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="138" priority="25" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P2,1)&lt;=6,FLOOR(P2,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="timePeriod" dxfId="143" priority="20" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="137" priority="26" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P5,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P5,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="142" priority="21" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="136" priority="27" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P5,1)&lt;=6,FLOOR(P5,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="141" priority="22" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="135" priority="28" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P5,1)&lt;=6,FLOOR(P5,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="timePeriod" dxfId="140" priority="23" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="134" priority="29" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P5,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P5,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="139" priority="24" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="133" priority="30" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P5,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P5,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="138" priority="25" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="132" priority="31" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P5,1)&lt;=6,FLOOR(P5,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4">
-    <cfRule type="timePeriod" dxfId="137" priority="26" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="131" priority="32" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P4,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P4,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="136" priority="27" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="130" priority="33" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P4,1)&lt;=6,FLOOR(P4,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="135" priority="28" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="129" priority="34" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P4,1)&lt;=6,FLOOR(P4,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4">
-    <cfRule type="timePeriod" dxfId="134" priority="29" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="128" priority="35" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P4,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P4,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="133" priority="30" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="127" priority="36" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P4,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P4,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="132" priority="31" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="126" priority="37" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P4,1)&lt;=6,FLOOR(P4,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3">
-    <cfRule type="timePeriod" dxfId="131" priority="32" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="125" priority="38" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P3,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P3,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="130" priority="33" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="124" priority="39" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P3,1)&lt;=6,FLOOR(P3,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="129" priority="34" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="123" priority="40" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P3,1)&lt;=6,FLOOR(P3,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3">
-    <cfRule type="timePeriod" dxfId="128" priority="35" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="122" priority="41" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P3,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P3,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="127" priority="36" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="121" priority="42" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P3,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P3,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="126" priority="37" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="120" priority="43" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P3,1)&lt;=6,FLOOR(P3,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P7">
-    <cfRule type="timePeriod" dxfId="125" priority="38" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="119" priority="44" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P7,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P7,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="124" priority="39" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="118" priority="45" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P7,1)&lt;=6,FLOOR(P7,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="123" priority="40" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="117" priority="46" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P7,1)&lt;=6,FLOOR(P7,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P7">
-    <cfRule type="timePeriod" dxfId="122" priority="41" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="116" priority="47" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P7,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P7,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="121" priority="42" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="115" priority="48" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P7,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P7,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="120" priority="43" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="114" priority="49" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P7,1)&lt;=6,FLOOR(P7,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P6">
-    <cfRule type="timePeriod" dxfId="119" priority="44" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="113" priority="50" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P6,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P6,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="118" priority="45" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="112" priority="51" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P6,1)&lt;=6,FLOOR(P6,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="117" priority="46" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="111" priority="52" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P6,1)&lt;=6,FLOOR(P6,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P6">
-    <cfRule type="timePeriod" dxfId="116" priority="47" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="110" priority="53" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P6,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P6,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="115" priority="48" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="109" priority="54" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P6,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P6,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="114" priority="49" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="108" priority="55" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P6,1)&lt;=6,FLOOR(P6,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P8">
-    <cfRule type="timePeriod" dxfId="113" priority="50" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="107" priority="56" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P8,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P8,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="112" priority="51" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="106" priority="57" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P8,1)&lt;=6,FLOOR(P8,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="111" priority="52" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="105" priority="58" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P8,1)&lt;=6,FLOOR(P8,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P8">
-    <cfRule type="timePeriod" dxfId="110" priority="53" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="104" priority="59" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P8,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P8,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="109" priority="54" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="103" priority="60" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P8,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P8,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="108" priority="55" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="102" priority="61" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P8,1)&lt;=6,FLOOR(P8,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P10">
-    <cfRule type="timePeriod" dxfId="107" priority="56" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="101" priority="62" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P10,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P10,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="106" priority="57" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="100" priority="63" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P10,1)&lt;=6,FLOOR(P10,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="105" priority="58" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="99" priority="64" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P10,1)&lt;=6,FLOOR(P10,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P10">
-    <cfRule type="timePeriod" dxfId="104" priority="59" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="98" priority="65" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P10,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P10,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="103" priority="60" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="97" priority="66" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P10,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P10,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="102" priority="61" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="96" priority="67" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P10,1)&lt;=6,FLOOR(P10,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P9">
-    <cfRule type="timePeriod" dxfId="101" priority="62" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="95" priority="68" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P9,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P9,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="100" priority="63" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="94" priority="69" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P9,1)&lt;=6,FLOOR(P9,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="99" priority="64" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="93" priority="70" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P9,1)&lt;=6,FLOOR(P9,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P9">
-    <cfRule type="timePeriod" dxfId="98" priority="65" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="92" priority="71" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P9,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P9,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="97" priority="66" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="91" priority="72" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P9,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P9,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="96" priority="67" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="90" priority="73" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P9,1)&lt;=6,FLOOR(P9,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P12">
-    <cfRule type="timePeriod" dxfId="95" priority="68" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="89" priority="74" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P12,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P12,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="94" priority="69" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="88" priority="75" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P12,1)&lt;=6,FLOOR(P12,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="93" priority="70" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="87" priority="76" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P12,1)&lt;=6,FLOOR(P12,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P12">
-    <cfRule type="timePeriod" dxfId="92" priority="71" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="86" priority="77" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P12,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P12,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="91" priority="72" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="85" priority="78" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P12,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P12,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="90" priority="73" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="84" priority="79" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P12,1)&lt;=6,FLOOR(P12,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P11">
-    <cfRule type="timePeriod" dxfId="89" priority="74" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="83" priority="80" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P11,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P11,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="88" priority="75" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="82" priority="81" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P11,1)&lt;=6,FLOOR(P11,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="87" priority="76" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="81" priority="82" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P11,1)&lt;=6,FLOOR(P11,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P11">
-    <cfRule type="timePeriod" dxfId="86" priority="77" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="80" priority="83" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P11,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P11,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="85" priority="78" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="79" priority="84" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P11,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P11,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="84" priority="79" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="78" priority="85" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P11,1)&lt;=6,FLOOR(P11,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P24">
-    <cfRule type="timePeriod" dxfId="83" priority="80" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="77" priority="86" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P24,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P24,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="82" priority="81" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="76" priority="87" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P24,1)&lt;=6,FLOOR(P24,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="81" priority="82" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="75" priority="88" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P24,1)&lt;=6,FLOOR(P24,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P24">
-    <cfRule type="timePeriod" dxfId="80" priority="83" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="74" priority="89" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P24,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P24,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="79" priority="84" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="73" priority="90" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P24,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P24,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="78" priority="85" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="72" priority="91" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P24,1)&lt;=6,FLOOR(P24,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16">
-    <cfRule type="timePeriod" dxfId="77" priority="86" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="71" priority="92" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="76" priority="87" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="70" priority="93" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P16,1)&lt;=6,FLOOR(P16,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="75" priority="88" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="69" priority="94" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P16,1)&lt;=6,FLOOR(P16,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16">
-    <cfRule type="timePeriod" dxfId="74" priority="89" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="68" priority="95" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P16,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P16,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="73" priority="90" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="67" priority="96" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="72" priority="91" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="66" priority="97" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P16,1)&lt;=6,FLOOR(P16,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P13">
-    <cfRule type="timePeriod" dxfId="71" priority="92" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="65" priority="98" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P13,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P13,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="70" priority="93" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="64" priority="99" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P13,1)&lt;=6,FLOOR(P13,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="69" priority="94" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="63" priority="100" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P13,1)&lt;=6,FLOOR(P13,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P13">
-    <cfRule type="timePeriod" dxfId="68" priority="95" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="62" priority="101" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P13,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P13,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="67" priority="96" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="61" priority="102" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P13,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P13,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="66" priority="97" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="60" priority="103" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P13,1)&lt;=6,FLOOR(P13,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17">
-    <cfRule type="timePeriod" dxfId="65" priority="98" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="59" priority="104" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P17,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P17,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="64" priority="99" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="58" priority="105" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P17,1)&lt;=6,FLOOR(P17,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="63" priority="100" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="57" priority="106" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P17,1)&lt;=6,FLOOR(P17,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17">
-    <cfRule type="timePeriod" dxfId="62" priority="101" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="56" priority="107" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P17,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P17,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="61" priority="102" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="55" priority="108" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P17,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P17,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="60" priority="103" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="54" priority="109" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P17,1)&lt;=6,FLOOR(P17,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P20">
-    <cfRule type="timePeriod" dxfId="59" priority="104" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="53" priority="110" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P20,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P20,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="58" priority="105" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="52" priority="111" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P20,1)&lt;=6,FLOOR(P20,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="57" priority="106" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="51" priority="112" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P20,1)&lt;=6,FLOOR(P20,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P20">
-    <cfRule type="timePeriod" dxfId="56" priority="107" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="50" priority="113" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P20,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P20,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="55" priority="108" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="49" priority="114" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P20,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P20,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="54" priority="109" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="48" priority="115" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P20,1)&lt;=6,FLOOR(P20,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P23">
-    <cfRule type="timePeriod" dxfId="53" priority="110" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="47" priority="116" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P23,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P23,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="52" priority="111" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="46" priority="117" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P23,1)&lt;=6,FLOOR(P23,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="51" priority="112" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="45" priority="118" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P23,1)&lt;=6,FLOOR(P23,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P23">
-    <cfRule type="timePeriod" dxfId="50" priority="113" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="44" priority="119" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P23,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P23,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="49" priority="114" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="43" priority="120" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P23,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P23,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="48" priority="115" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="42" priority="121" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P23,1)&lt;=6,FLOOR(P23,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P25">
-    <cfRule type="timePeriod" dxfId="47" priority="116" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="41" priority="122" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P25,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P25,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="46" priority="117" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="40" priority="123" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P25,1)&lt;=6,FLOOR(P25,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="45" priority="118" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="39" priority="124" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P25,1)&lt;=6,FLOOR(P25,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P25">
-    <cfRule type="timePeriod" dxfId="44" priority="119" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="38" priority="125" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P25,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P25,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="43" priority="120" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="37" priority="126" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P25,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P25,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="42" priority="121" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="36" priority="127" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P25,1)&lt;=6,FLOOR(P25,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="P29">
+    <cfRule type="timePeriod" dxfId="35" priority="134" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P29,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P29,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="34" priority="135" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P29,1)&lt;=6,FLOOR(P29,1)&lt;=TODAY())</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="33" priority="136" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P29,1)&lt;=6,FLOOR(P29,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P29">
+    <cfRule type="timePeriod" dxfId="32" priority="137" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(P29,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P29,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="31" priority="138" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P29,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P29,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="30" priority="139" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P29,1)&lt;=6,FLOOR(P29,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P28">
+    <cfRule type="timePeriod" dxfId="29" priority="140" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P28,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P28,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="28" priority="141" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P28,1)&lt;=6,FLOOR(P28,1)&lt;=TODAY())</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="27" priority="142" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P28,1)&lt;=6,FLOOR(P28,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P28">
+    <cfRule type="timePeriod" dxfId="26" priority="143" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(P28,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P28,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="25" priority="144" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P28,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P28,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="24" priority="145" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P28,1)&lt;=6,FLOOR(P28,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P33">
+    <cfRule type="timePeriod" dxfId="23" priority="146" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P33,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P33,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="22" priority="147" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P33,1)&lt;=6,FLOOR(P33,1)&lt;=TODAY())</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="21" priority="148" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P33,1)&lt;=6,FLOOR(P33,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P33">
+    <cfRule type="timePeriod" dxfId="20" priority="149" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(P33,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P33,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="19" priority="150" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P33,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P33,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="18" priority="151" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P33,1)&lt;=6,FLOOR(P33,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P30">
+    <cfRule type="timePeriod" dxfId="17" priority="7" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P30,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P30,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="16" priority="8" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P30,1)&lt;=6,FLOOR(P30,1)&lt;=TODAY())</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="15" priority="9" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P30,1)&lt;=6,FLOOR(P30,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P30">
+    <cfRule type="timePeriod" dxfId="14" priority="10" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(P30,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P30,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="13" priority="11" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P30,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P30,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="12" priority="12" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P30,1)&lt;=6,FLOOR(P30,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P31">
+    <cfRule type="timePeriod" dxfId="11" priority="13" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P31,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P31,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="10" priority="14" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P31,1)&lt;=6,FLOOR(P31,1)&lt;=TODAY())</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="9" priority="15" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P31,1)&lt;=6,FLOOR(P31,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P31">
+    <cfRule type="timePeriod" dxfId="8" priority="16" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(P31,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P31,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="7" priority="17" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(P31,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P31,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="6" priority="18" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(P31,1)&lt;=6,FLOOR(P31,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="P32">
-    <cfRule type="timePeriod" dxfId="41" priority="122" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="5" priority="1" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P32,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P32,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="40" priority="123" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="4" priority="2" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P32,1)&lt;=6,FLOOR(P32,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="39" priority="124" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="3" priority="3" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P32,1)&lt;=6,FLOOR(P32,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P32">
-    <cfRule type="timePeriod" dxfId="38" priority="125" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="2" priority="4" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(P32,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P32,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="37" priority="126" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="1" priority="5" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(P32,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P32,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="36" priority="127" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="0" priority="6" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(P32,1)&lt;=6,FLOOR(P32,1)&lt;=TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P29">
-    <cfRule type="timePeriod" dxfId="35" priority="128" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(P29,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P29,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="34" priority="129" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P29,1)&lt;=6,FLOOR(P29,1)&lt;=TODAY())</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="33" priority="130" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P29,1)&lt;=6,FLOOR(P29,1)&lt;=TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P29">
-    <cfRule type="timePeriod" dxfId="32" priority="131" timePeriod="thisWeek">
-      <formula>AND(TODAY()-ROUNDDOWN(P29,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P29,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="31" priority="132" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(P29,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P29,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="30" priority="133" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P29,1)&lt;=6,FLOOR(P29,1)&lt;=TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P28">
-    <cfRule type="timePeriod" dxfId="29" priority="134" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(P28,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P28,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="28" priority="135" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P28,1)&lt;=6,FLOOR(P28,1)&lt;=TODAY())</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="27" priority="136" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P28,1)&lt;=6,FLOOR(P28,1)&lt;=TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P28">
-    <cfRule type="timePeriod" dxfId="26" priority="137" timePeriod="thisWeek">
-      <formula>AND(TODAY()-ROUNDDOWN(P28,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P28,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="25" priority="138" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(P28,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P28,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="24" priority="139" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P28,1)&lt;=6,FLOOR(P28,1)&lt;=TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P34">
-    <cfRule type="timePeriod" dxfId="23" priority="140" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(P34,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P34,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="22" priority="141" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P34,1)&lt;=6,FLOOR(P34,1)&lt;=TODAY())</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="21" priority="142" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P34,1)&lt;=6,FLOOR(P34,1)&lt;=TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P34">
-    <cfRule type="timePeriod" dxfId="20" priority="143" timePeriod="thisWeek">
-      <formula>AND(TODAY()-ROUNDDOWN(P34,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P34,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="19" priority="144" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(P34,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P34,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="18" priority="145" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P34,1)&lt;=6,FLOOR(P34,1)&lt;=TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P33">
-    <cfRule type="timePeriod" dxfId="17" priority="146" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(P33,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P33,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="16" priority="147" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P33,1)&lt;=6,FLOOR(P33,1)&lt;=TODAY())</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="15" priority="148" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P33,1)&lt;=6,FLOOR(P33,1)&lt;=TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P33">
-    <cfRule type="timePeriod" dxfId="14" priority="149" timePeriod="thisWeek">
-      <formula>AND(TODAY()-ROUNDDOWN(P33,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P33,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="13" priority="150" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(P33,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P33,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="12" priority="151" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P33,1)&lt;=6,FLOOR(P33,1)&lt;=TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P30">
-    <cfRule type="timePeriod" dxfId="11" priority="1" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(P30,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P30,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="10" priority="2" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P30,1)&lt;=6,FLOOR(P30,1)&lt;=TODAY())</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="9" priority="3" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P30,1)&lt;=6,FLOOR(P30,1)&lt;=TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P30">
-    <cfRule type="timePeriod" dxfId="8" priority="4" timePeriod="thisWeek">
-      <formula>AND(TODAY()-ROUNDDOWN(P30,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P30,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="7" priority="5" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(P30,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P30,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="6" priority="6" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P30,1)&lt;=6,FLOOR(P30,1)&lt;=TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P31">
-    <cfRule type="timePeriod" dxfId="5" priority="7" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(P31,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P31,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="4" priority="8" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P31,1)&lt;=6,FLOOR(P31,1)&lt;=TODAY())</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="3" priority="9" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P31,1)&lt;=6,FLOOR(P31,1)&lt;=TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P31">
-    <cfRule type="timePeriod" dxfId="2" priority="10" timePeriod="thisWeek">
-      <formula>AND(TODAY()-ROUNDDOWN(P31,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(P31,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="1" priority="11" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(P31,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(P31,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="0" priority="12" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(P31,1)&lt;=6,FLOOR(P31,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>